<commit_message>
update aacar bolew sdcol
aacar 6 attempt workaround for missing axon terminal in epicardium

bolew 13-29 workaround for https://github.com/open-physiology/open-physiology-viewer/issues/209
      3 correct housingLyph for dendrite

sdcol b fix layer inversion when passing through white matter
      add general reference about enteric inhibitory motor neurons
</commit_message>
<xml_diff>
--- a/models/sawg-distal-colon/source/sawg-distal-colon.xlsx
+++ b/models/sawg-distal-colon/source/sawg-distal-colon.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="1067">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1656" uniqueCount="1075">
   <si>
     <t>id</t>
   </si>
@@ -1165,7 +1165,7 @@
     <t>ns5</t>
   </si>
   <si>
-    <t>6,0,0,0,0,0</t>
+    <t>6,13,0,0,0,0</t>
   </si>
   <si>
     <t>S4, S4, S16, S39, S27, S33</t>
@@ -3049,6 +3049,9 @@
     <t>ilxtr:neuron-type-sdcol-j</t>
   </si>
   <si>
+    <t>enteric excitatory motor neuron</t>
+  </si>
+  <si>
     <t>Neuron j2</t>
   </si>
   <si>
@@ -3067,6 +3070,12 @@
     <t>ilxtr:neuron-type-sdcol-l</t>
   </si>
   <si>
+    <t>PMID:8601295</t>
+  </si>
+  <si>
+    <t>enteric NOS inhibitory motor neuron</t>
+  </si>
+  <si>
     <t>Neuron l2</t>
   </si>
   <si>
@@ -3079,6 +3088,9 @@
     <t>ilxtr:neuron-type-sdcol-m</t>
   </si>
   <si>
+    <t>enteric intrinsic primary afferent neuron</t>
+  </si>
+  <si>
     <t>Neuron n</t>
   </si>
   <si>
@@ -3091,7 +3103,7 @@
     <t>ilxtr:neuron-type-sdcol-o</t>
   </si>
   <si>
-    <t xml:space="preserve">vasodilatory motor neuron </t>
+    <t>enteric vasodilatory motor neuron</t>
   </si>
   <si>
     <t>Neuron p</t>
@@ -3100,7 +3112,7 @@
     <t>ilxtr:neuron-type-sdcol-p</t>
   </si>
   <si>
-    <t>secretomotor neuron</t>
+    <t>enteric secretomotor neuron</t>
   </si>
   <si>
     <t>Neuron q</t>
@@ -3157,6 +3169,12 @@
     <t>https://pubmed.ncbi.nlm.nih.gov/4044909/</t>
   </si>
   <si>
+    <t>from Tom for inhibitory motor neuron</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/8601295/</t>
+  </si>
+  <si>
     <t>notes</t>
   </si>
   <si>
@@ -3263,13 +3281,19 @@
   </si>
   <si>
     <t>http://uri.interlex.org/tgbugs/uris/readable/</t>
+  </si>
+  <si>
+    <t>doi</t>
+  </si>
+  <si>
+    <t>https://doi.org/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -3383,6 +3407,10 @@
       <u/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
     <font>
       <u/>
@@ -3506,7 +3534,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="170">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -4000,6 +4028,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -4310,51 +4341,51 @@
         <v>1</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>1031</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="164" t="s">
-        <v>1032</v>
+        <v>1038</v>
       </c>
       <c r="B2" s="165" t="s">
-        <v>1033</v>
+        <v>1039</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>1034</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="164" t="s">
-        <v>1035</v>
+        <v>1041</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>1036</v>
+        <v>1042</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>1034</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="164" t="s">
-        <v>1037</v>
+        <v>1043</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>1038</v>
+        <v>1044</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>1034</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="163" t="s">
-        <v>1039</v>
+        <v>1045</v>
       </c>
       <c r="B5" s="142" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>1040</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>1034</v>
       </c>
     </row>
   </sheetData>
@@ -4383,106 +4414,114 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="166" t="s">
-        <v>1041</v>
+        <v>1047</v>
       </c>
       <c r="B1" s="166" t="s">
-        <v>1042</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="167" t="s">
-        <v>1043</v>
+        <v>1049</v>
       </c>
       <c r="B2" s="168" t="s">
-        <v>1044</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="167" t="s">
-        <v>1045</v>
+        <v>1051</v>
       </c>
       <c r="B3" s="168" t="s">
-        <v>1046</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="167" t="s">
-        <v>1047</v>
+        <v>1053</v>
       </c>
       <c r="B4" s="168" t="s">
-        <v>1048</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="167" t="s">
-        <v>1049</v>
+        <v>1055</v>
       </c>
       <c r="B5" s="168" t="s">
-        <v>1050</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="167" t="s">
-        <v>1051</v>
+        <v>1057</v>
       </c>
       <c r="B6" s="168" t="s">
-        <v>1052</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="167" t="s">
-        <v>1053</v>
+        <v>1059</v>
       </c>
       <c r="B7" s="168" t="s">
-        <v>1054</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="167" t="s">
-        <v>1055</v>
+        <v>1061</v>
       </c>
       <c r="B8" s="168" t="s">
-        <v>1056</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="167" t="s">
-        <v>1057</v>
+        <v>1063</v>
       </c>
       <c r="B9" s="168" t="s">
-        <v>1058</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="167" t="s">
-        <v>1059</v>
+        <v>1065</v>
       </c>
       <c r="B10" s="168" t="s">
-        <v>1060</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="167" t="s">
-        <v>1061</v>
+        <v>1067</v>
       </c>
       <c r="B11" s="168" t="s">
-        <v>1062</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="167" t="s">
-        <v>1063</v>
+        <v>1069</v>
       </c>
       <c r="B12" s="168" t="s">
-        <v>1064</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="167" t="s">
-        <v>1065</v>
+        <v>1071</v>
       </c>
       <c r="B13" s="168" t="s">
-        <v>1066</v>
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="16" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B14" s="169" t="s">
+        <v>1074</v>
       </c>
     </row>
   </sheetData>
@@ -4499,8 +4538,9 @@
     <hyperlink r:id="rId10" ref="B11"/>
     <hyperlink r:id="rId11" ref="B12"/>
     <hyperlink r:id="rId12" ref="B13"/>
+    <hyperlink r:id="rId13" ref="B14"/>
   </hyperlinks>
-  <drawing r:id="rId13"/>
+  <drawing r:id="rId14"/>
 </worksheet>
 </file>
 
@@ -12687,7 +12727,7 @@
       <c r="H9" s="153"/>
       <c r="I9" s="153"/>
       <c r="J9" s="161" t="s">
-        <v>891</v>
+        <v>995</v>
       </c>
     </row>
     <row r="10">
@@ -12695,10 +12735,10 @@
         <v>287</v>
       </c>
       <c r="B10" s="153" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="C10" s="153" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="D10" s="153"/>
       <c r="E10" s="158"/>
@@ -12707,7 +12747,7 @@
       <c r="H10" s="153"/>
       <c r="I10" s="153"/>
       <c r="J10" s="161" t="s">
-        <v>891</v>
+        <v>995</v>
       </c>
     </row>
     <row r="11">
@@ -12715,10 +12755,10 @@
         <v>290</v>
       </c>
       <c r="B11" s="153" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="C11" s="153" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="D11" s="153"/>
       <c r="E11" s="158"/>
@@ -12735,19 +12775,21 @@
         <v>293</v>
       </c>
       <c r="B12" s="153" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="C12" s="153" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="D12" s="153"/>
       <c r="E12" s="158"/>
       <c r="F12" s="155"/>
       <c r="G12" s="153"/>
       <c r="H12" s="153"/>
-      <c r="I12" s="153"/>
+      <c r="I12" s="16" t="s">
+        <v>1002</v>
+      </c>
       <c r="J12" s="157" t="s">
-        <v>893</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="13">
@@ -12755,19 +12797,21 @@
         <v>296</v>
       </c>
       <c r="B13" s="153" t="s">
-        <v>1001</v>
+        <v>1004</v>
       </c>
       <c r="C13" s="153" t="s">
-        <v>1002</v>
+        <v>1005</v>
       </c>
       <c r="D13" s="153"/>
       <c r="E13" s="158"/>
       <c r="F13" s="156"/>
       <c r="G13" s="153"/>
       <c r="H13" s="153"/>
-      <c r="I13" s="153"/>
+      <c r="I13" s="16" t="s">
+        <v>1002</v>
+      </c>
       <c r="J13" s="157" t="s">
-        <v>893</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="14">
@@ -12775,19 +12819,18 @@
         <v>299</v>
       </c>
       <c r="B14" s="153" t="s">
-        <v>1003</v>
+        <v>1006</v>
       </c>
       <c r="C14" s="153" t="s">
-        <v>1004</v>
+        <v>1007</v>
       </c>
       <c r="D14" s="153"/>
       <c r="E14" s="158"/>
       <c r="F14" s="156"/>
       <c r="G14" s="153"/>
       <c r="H14" s="153"/>
-      <c r="I14" s="152"/>
       <c r="J14" s="160" t="s">
-        <v>895</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="15">
@@ -12795,19 +12838,18 @@
         <v>302</v>
       </c>
       <c r="B15" s="153" t="s">
-        <v>1005</v>
+        <v>1009</v>
       </c>
       <c r="C15" s="153" t="s">
-        <v>1006</v>
+        <v>1010</v>
       </c>
       <c r="D15" s="153"/>
       <c r="E15" s="158"/>
       <c r="F15" s="156"/>
       <c r="G15" s="153"/>
       <c r="H15" s="153"/>
-      <c r="I15" s="152"/>
       <c r="J15" s="160" t="s">
-        <v>895</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="16">
@@ -12815,10 +12857,10 @@
         <v>305</v>
       </c>
       <c r="B16" s="153" t="s">
-        <v>1007</v>
+        <v>1011</v>
       </c>
       <c r="C16" s="153" t="s">
-        <v>1008</v>
+        <v>1012</v>
       </c>
       <c r="D16" s="153"/>
       <c r="E16" s="158"/>
@@ -12827,7 +12869,7 @@
       <c r="H16" s="153"/>
       <c r="I16" s="153"/>
       <c r="J16" s="153" t="s">
-        <v>1009</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="17">
@@ -12835,10 +12877,10 @@
         <v>308</v>
       </c>
       <c r="B17" s="153" t="s">
-        <v>1010</v>
+        <v>1014</v>
       </c>
       <c r="C17" s="153" t="s">
-        <v>1011</v>
+        <v>1015</v>
       </c>
       <c r="D17" s="153"/>
       <c r="E17" s="158"/>
@@ -12847,7 +12889,7 @@
       <c r="H17" s="153"/>
       <c r="I17" s="152"/>
       <c r="J17" s="162" t="s">
-        <v>1012</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="18">
@@ -12855,10 +12897,10 @@
         <v>311</v>
       </c>
       <c r="B18" s="153" t="s">
-        <v>1013</v>
+        <v>1017</v>
       </c>
       <c r="C18" s="153" t="s">
-        <v>1014</v>
+        <v>1018</v>
       </c>
       <c r="D18" s="153"/>
       <c r="E18" s="158"/>
@@ -12867,7 +12909,7 @@
       <c r="H18" s="153"/>
       <c r="I18" s="152"/>
       <c r="J18" s="162" t="s">
-        <v>1015</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="19">
@@ -12875,10 +12917,10 @@
         <v>314</v>
       </c>
       <c r="B19" s="153" t="s">
-        <v>1016</v>
+        <v>1020</v>
       </c>
       <c r="C19" s="153" t="s">
-        <v>1017</v>
+        <v>1021</v>
       </c>
       <c r="D19" s="153"/>
       <c r="E19" s="158"/>
@@ -12887,15 +12929,15 @@
       <c r="H19" s="153"/>
       <c r="I19" s="152"/>
       <c r="J19" s="162" t="s">
-        <v>1018</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="158" t="s">
-        <v>1019</v>
+        <v>1023</v>
       </c>
       <c r="B20" s="153" t="s">
-        <v>1020</v>
+        <v>1024</v>
       </c>
       <c r="C20" s="158"/>
       <c r="D20" s="158" t="s">
@@ -12927,49 +12969,60 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+      <c r="A1" s="1">
+        <v>1.0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1021</v>
+        <v>1025</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1022</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="16" t="s">
-        <v>1023</v>
+        <v>1027</v>
       </c>
       <c r="C2" s="163" t="s">
-        <v>1024</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="16" t="s">
-        <v>1025</v>
+        <v>1029</v>
       </c>
       <c r="C3" s="163" t="s">
-        <v>1026</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="16" t="s">
-        <v>1027</v>
+        <v>1031</v>
       </c>
       <c r="C4" s="163" t="s">
-        <v>1028</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="16" t="s">
-        <v>1029</v>
+        <v>1033</v>
       </c>
       <c r="C5" s="163" t="s">
-        <v>1030</v>
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="16" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C6" s="163" t="s">
+        <v>1036</v>
       </c>
     </row>
   </sheetData>
@@ -12978,7 +13031,8 @@
     <hyperlink r:id="rId2" ref="C3"/>
     <hyperlink r:id="rId3" ref="C4"/>
     <hyperlink r:id="rId4" ref="C5"/>
+    <hyperlink r:id="rId5" ref="C6"/>
   </hyperlinks>
-  <drawing r:id="rId5"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sdcol fix references id column typo
</commit_message>
<xml_diff>
--- a/models/sawg-distal-colon/source/sawg-distal-colon.xlsx
+++ b/models/sawg-distal-colon/source/sawg-distal-colon.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1656" uniqueCount="1075">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1657" uniqueCount="1075">
   <si>
     <t>id</t>
   </si>
@@ -12969,8 +12969,8 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1">
-        <v>1.0</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
sdcol f and o correct layer from blood to wall
sdcol f also fix incorrect use of non-existent SAO ontology ids that
were the result of the sheets program trying to be smart and
autoincrement the numbers :/
</commit_message>
<xml_diff>
--- a/models/sawg-distal-colon/source/sawg-distal-colon.xlsx
+++ b/models/sawg-distal-colon/source/sawg-distal-colon.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
     <author/>
   </authors>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1657" uniqueCount="1075">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1657" uniqueCount="1069">
   <si>
     <t>id</t>
   </si>
@@ -1777,9 +1777,6 @@
     <t>Axon chain of Symp postganglionic neuron in Arteriole in longitudinal muscle layer of colon _Neuron F (sdcol)</t>
   </si>
   <si>
-    <t>SAO:1770195790</t>
-  </si>
-  <si>
     <t>f-term-root-S60</t>
   </si>
   <si>
@@ -1792,9 +1789,6 @@
     <t>Axon chain of Symp postganglionic neuron in Arteriole in serosa of colon _Neuron F (sdcol)</t>
   </si>
   <si>
-    <t>SAO:1770195791</t>
-  </si>
-  <si>
     <t>f-term-root-S61</t>
   </si>
   <si>
@@ -1807,9 +1801,6 @@
     <t>Axon chain of Symp postganglionic neuron in Arteriole in myenteric nerve plexus in colon_NeuronF (sdcol)</t>
   </si>
   <si>
-    <t>SAO:1770195792</t>
-  </si>
-  <si>
     <t>f-term-root-S62</t>
   </si>
   <si>
@@ -1822,9 +1813,6 @@
     <t>Axon chain of Symp postganglionic neuron in Arteriole in submucosal nerve plexus of colon_Neuron F (sdcol)</t>
   </si>
   <si>
-    <t>SAO:1770195793</t>
-  </si>
-  <si>
     <t>f-term-root-S63</t>
   </si>
   <si>
@@ -1837,9 +1825,6 @@
     <t>Axon chain of Symp postganglionic neuron in Arteriole in circular muscle layer in colon_Neuron F (sdcol)</t>
   </si>
   <si>
-    <t>SAO:1770195794</t>
-  </si>
-  <si>
     <t>f-term-root-S64</t>
   </si>
   <si>
@@ -1852,9 +1837,6 @@
     <t>Axon chain of Symp postganglionic neuron in Arteriole in lamina propria of mucosa of colon _Neuron F (sdcol)</t>
   </si>
   <si>
-    <t>SAO:1770195795</t>
-  </si>
-  <si>
     <t>f-term-root-S65</t>
   </si>
   <si>
@@ -2194,7 +2176,7 @@
     <t>ns75</t>
   </si>
   <si>
-    <t>3,0</t>
+    <t>3,1</t>
   </si>
   <si>
     <t>S42,S64</t>
@@ -3534,7 +3516,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="170">
+  <cellXfs count="171">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3868,6 +3850,9 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="10" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -4341,51 +4326,51 @@
         <v>1</v>
       </c>
       <c r="C1" s="18" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="165" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B2" s="166" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="165" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="165" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="164" t="s">
+      <c r="B4" s="18" t="s">
         <v>1038</v>
       </c>
-      <c r="B2" s="165" t="s">
+      <c r="C4" s="16" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="164" t="s">
         <v>1039</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="B5" s="143" t="s">
         <v>1040</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="164" t="s">
-        <v>1041</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>1042</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>1040</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="164" t="s">
-        <v>1043</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>1044</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>1040</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="163" t="s">
-        <v>1045</v>
-      </c>
-      <c r="B5" s="142" t="s">
-        <v>1046</v>
-      </c>
       <c r="C5" s="16" t="s">
-        <v>1040</v>
+        <v>1034</v>
       </c>
     </row>
   </sheetData>
@@ -4413,115 +4398,115 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="166" t="s">
+      <c r="A1" s="167" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B1" s="167" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="168" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B2" s="169" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="168" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B3" s="169" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="168" t="s">
         <v>1047</v>
       </c>
-      <c r="B1" s="166" t="s">
+      <c r="B4" s="169" t="s">
         <v>1048</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="167" t="s">
+    <row r="5">
+      <c r="A5" s="168" t="s">
         <v>1049</v>
       </c>
-      <c r="B2" s="168" t="s">
+      <c r="B5" s="169" t="s">
         <v>1050</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="167" t="s">
+    <row r="6">
+      <c r="A6" s="168" t="s">
         <v>1051</v>
       </c>
-      <c r="B3" s="168" t="s">
+      <c r="B6" s="169" t="s">
         <v>1052</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="167" t="s">
+    <row r="7">
+      <c r="A7" s="168" t="s">
         <v>1053</v>
       </c>
-      <c r="B4" s="168" t="s">
+      <c r="B7" s="169" t="s">
         <v>1054</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="167" t="s">
+    <row r="8">
+      <c r="A8" s="168" t="s">
         <v>1055</v>
       </c>
-      <c r="B5" s="168" t="s">
+      <c r="B8" s="169" t="s">
         <v>1056</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="167" t="s">
+    <row r="9">
+      <c r="A9" s="168" t="s">
         <v>1057</v>
       </c>
-      <c r="B6" s="168" t="s">
+      <c r="B9" s="169" t="s">
         <v>1058</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="167" t="s">
+    <row r="10">
+      <c r="A10" s="168" t="s">
         <v>1059</v>
       </c>
-      <c r="B7" s="168" t="s">
+      <c r="B10" s="169" t="s">
         <v>1060</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="167" t="s">
+    <row r="11">
+      <c r="A11" s="168" t="s">
         <v>1061</v>
       </c>
-      <c r="B8" s="168" t="s">
+      <c r="B11" s="169" t="s">
         <v>1062</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="167" t="s">
+    <row r="12">
+      <c r="A12" s="168" t="s">
         <v>1063</v>
       </c>
-      <c r="B9" s="168" t="s">
+      <c r="B12" s="169" t="s">
         <v>1064</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="167" t="s">
+    <row r="13">
+      <c r="A13" s="168" t="s">
         <v>1065</v>
       </c>
-      <c r="B10" s="168" t="s">
+      <c r="B13" s="169" t="s">
         <v>1066</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="167" t="s">
-        <v>1067</v>
-      </c>
-      <c r="B11" s="168" t="s">
-        <v>1068</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="167" t="s">
-        <v>1069</v>
-      </c>
-      <c r="B12" s="168" t="s">
-        <v>1070</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="167" t="s">
-        <v>1071</v>
-      </c>
-      <c r="B13" s="168" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="16" t="s">
-        <v>1073</v>
-      </c>
-      <c r="B14" s="169" t="s">
-        <v>1074</v>
+        <v>1067</v>
+      </c>
+      <c r="B14" s="170" t="s">
+        <v>1068</v>
       </c>
     </row>
   </sheetData>
@@ -9522,15 +9507,15 @@
       <c r="B63" s="105" t="s">
         <v>570</v>
       </c>
-      <c r="C63" s="99" t="s">
-        <v>571</v>
+      <c r="C63" s="113" t="s">
+        <v>364</v>
       </c>
       <c r="D63" s="107"/>
       <c r="E63" s="90" t="s">
+        <v>571</v>
+      </c>
+      <c r="F63" s="90" t="s">
         <v>572</v>
-      </c>
-      <c r="F63" s="90" t="s">
-        <v>573</v>
       </c>
       <c r="G63" s="107"/>
       <c r="H63" s="90" t="s">
@@ -9539,30 +9524,30 @@
       <c r="I63" s="107"/>
       <c r="J63" s="19"/>
       <c r="K63" s="97">
-        <v>0.0</v>
-      </c>
-      <c r="L63" s="113" t="s">
+        <v>1.0</v>
+      </c>
+      <c r="L63" s="114" t="s">
         <v>168</v>
       </c>
-      <c r="M63" s="113"/>
-      <c r="N63" s="114"/>
+      <c r="M63" s="114"/>
+      <c r="N63" s="115"/>
     </row>
     <row r="64">
       <c r="A64" s="90" t="s">
+        <v>573</v>
+      </c>
+      <c r="B64" s="105" t="s">
         <v>574</v>
       </c>
-      <c r="B64" s="105" t="s">
-        <v>575</v>
-      </c>
-      <c r="C64" s="99" t="s">
-        <v>576</v>
+      <c r="C64" s="113" t="s">
+        <v>364</v>
       </c>
       <c r="D64" s="107"/>
       <c r="E64" s="90" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="F64" s="90" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="G64" s="107"/>
       <c r="H64" s="90" t="s">
@@ -9571,30 +9556,30 @@
       <c r="I64" s="107"/>
       <c r="J64" s="19"/>
       <c r="K64" s="97">
-        <v>0.0</v>
-      </c>
-      <c r="L64" s="113" t="s">
+        <v>1.0</v>
+      </c>
+      <c r="L64" s="114" t="s">
         <v>243</v>
       </c>
-      <c r="M64" s="113"/>
-      <c r="N64" s="114"/>
+      <c r="M64" s="114"/>
+      <c r="N64" s="115"/>
     </row>
     <row r="65">
       <c r="A65" s="90" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B65" s="105" t="s">
-        <v>580</v>
-      </c>
-      <c r="C65" s="99" t="s">
-        <v>581</v>
+        <v>578</v>
+      </c>
+      <c r="C65" s="113" t="s">
+        <v>364</v>
       </c>
       <c r="D65" s="107"/>
       <c r="E65" s="90" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="F65" s="90" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="G65" s="107"/>
       <c r="H65" s="90" t="s">
@@ -9603,30 +9588,30 @@
       <c r="I65" s="107"/>
       <c r="J65" s="19"/>
       <c r="K65" s="97">
-        <v>0.0</v>
-      </c>
-      <c r="L65" s="113" t="s">
+        <v>1.0</v>
+      </c>
+      <c r="L65" s="114" t="s">
         <v>164</v>
       </c>
-      <c r="M65" s="113"/>
-      <c r="N65" s="114"/>
+      <c r="M65" s="114"/>
+      <c r="N65" s="115"/>
     </row>
     <row r="66">
       <c r="A66" s="90" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="B66" s="105" t="s">
-        <v>585</v>
-      </c>
-      <c r="C66" s="99" t="s">
-        <v>586</v>
+        <v>582</v>
+      </c>
+      <c r="C66" s="113" t="s">
+        <v>364</v>
       </c>
       <c r="D66" s="107"/>
       <c r="E66" s="90" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="F66" s="90" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="G66" s="107"/>
       <c r="H66" s="90" t="s">
@@ -9635,30 +9620,30 @@
       <c r="I66" s="107"/>
       <c r="J66" s="19"/>
       <c r="K66" s="97">
-        <v>0.0</v>
-      </c>
-      <c r="L66" s="113" t="s">
+        <v>1.0</v>
+      </c>
+      <c r="L66" s="114" t="s">
         <v>248</v>
       </c>
-      <c r="M66" s="113"/>
-      <c r="N66" s="114"/>
+      <c r="M66" s="114"/>
+      <c r="N66" s="115"/>
     </row>
     <row r="67">
       <c r="A67" s="90" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="B67" s="105" t="s">
-        <v>590</v>
-      </c>
-      <c r="C67" s="99" t="s">
-        <v>591</v>
+        <v>586</v>
+      </c>
+      <c r="C67" s="113" t="s">
+        <v>364</v>
       </c>
       <c r="D67" s="107"/>
       <c r="E67" s="90" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="F67" s="90" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="G67" s="107"/>
       <c r="H67" s="90" t="s">
@@ -9667,30 +9652,30 @@
       <c r="I67" s="107"/>
       <c r="J67" s="19"/>
       <c r="K67" s="97">
-        <v>0.0</v>
-      </c>
-      <c r="L67" s="113" t="s">
+        <v>1.0</v>
+      </c>
+      <c r="L67" s="114" t="s">
         <v>181</v>
       </c>
-      <c r="M67" s="113"/>
-      <c r="N67" s="114"/>
+      <c r="M67" s="114"/>
+      <c r="N67" s="115"/>
     </row>
     <row r="68">
       <c r="A68" s="90" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="B68" s="105" t="s">
-        <v>595</v>
-      </c>
-      <c r="C68" s="99" t="s">
-        <v>596</v>
+        <v>590</v>
+      </c>
+      <c r="C68" s="113" t="s">
+        <v>364</v>
       </c>
       <c r="D68" s="107"/>
       <c r="E68" s="90" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="F68" s="90" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
       <c r="G68" s="107"/>
       <c r="H68" s="90" t="s">
@@ -9699,27 +9684,27 @@
       <c r="I68" s="107"/>
       <c r="J68" s="19"/>
       <c r="K68" s="97">
-        <v>0.0</v>
-      </c>
-      <c r="L68" s="113" t="s">
+        <v>1.0</v>
+      </c>
+      <c r="L68" s="114" t="s">
         <v>253</v>
       </c>
-      <c r="M68" s="113"/>
-      <c r="N68" s="114"/>
+      <c r="M68" s="114"/>
+      <c r="N68" s="115"/>
     </row>
     <row r="69">
       <c r="A69" s="104" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="B69" s="105" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="C69" s="106" t="s">
         <v>360</v>
       </c>
       <c r="D69" s="107"/>
       <c r="E69" s="90" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="F69" s="90"/>
       <c r="G69" s="107"/>
@@ -9731,28 +9716,28 @@
       <c r="K69" s="97">
         <v>0.0</v>
       </c>
-      <c r="L69" s="113" t="s">
+      <c r="L69" s="114" t="s">
         <v>151</v>
       </c>
-      <c r="M69" s="113"/>
-      <c r="N69" s="114"/>
+      <c r="M69" s="114"/>
+      <c r="N69" s="115"/>
     </row>
     <row r="70">
       <c r="A70" s="104" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="B70" s="105" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="C70" s="106" t="s">
         <v>364</v>
       </c>
       <c r="D70" s="107"/>
       <c r="E70" s="90" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="F70" s="90" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="G70" s="107"/>
       <c r="H70" s="90" t="s">
@@ -9761,29 +9746,29 @@
       <c r="I70" s="107"/>
       <c r="J70" s="19"/>
       <c r="K70" s="97" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="L70" s="108" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="M70" s="108" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="N70" s="19"/>
     </row>
     <row r="71">
       <c r="A71" s="82" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="B71" s="83" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
       <c r="C71" s="84" t="s">
         <v>360</v>
       </c>
       <c r="D71" s="87"/>
       <c r="E71" s="86" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
       <c r="F71" s="87"/>
       <c r="G71" s="87"/>
@@ -9803,20 +9788,20 @@
     </row>
     <row r="72">
       <c r="A72" s="82" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B72" s="83" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="C72" s="84" t="s">
         <v>364</v>
       </c>
       <c r="D72" s="87"/>
       <c r="E72" s="86" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="F72" s="86" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="G72" s="87"/>
       <c r="H72" s="86" t="s">
@@ -9825,27 +9810,27 @@
       <c r="I72" s="87"/>
       <c r="J72" s="89"/>
       <c r="K72" s="110" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="L72" s="98" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="M72" s="98"/>
       <c r="N72" s="89"/>
     </row>
     <row r="73">
       <c r="A73" s="15" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="B73" s="77" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="C73" s="99" t="s">
         <v>360</v>
       </c>
       <c r="D73" s="22"/>
       <c r="E73" s="4" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
       <c r="F73" s="22"/>
       <c r="G73" s="22"/>
@@ -9865,20 +9850,20 @@
     </row>
     <row r="74">
       <c r="A74" s="15" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
       <c r="B74" s="77" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="C74" s="99" t="s">
         <v>364</v>
       </c>
       <c r="D74" s="22"/>
       <c r="E74" s="4" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
       <c r="G74" s="22"/>
       <c r="H74" s="4" t="s">
@@ -9887,27 +9872,27 @@
       <c r="I74" s="22"/>
       <c r="J74" s="18"/>
       <c r="K74" s="102" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="L74" s="103" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
       <c r="M74" s="103"/>
       <c r="N74" s="18"/>
     </row>
     <row r="75">
       <c r="A75" s="82" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
       <c r="B75" s="83" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="C75" s="84" t="s">
         <v>360</v>
       </c>
       <c r="D75" s="87"/>
       <c r="E75" s="86" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="F75" s="87"/>
       <c r="G75" s="87"/>
@@ -9927,20 +9912,20 @@
     </row>
     <row r="76">
       <c r="A76" s="82" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="B76" s="83" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="C76" s="84" t="s">
         <v>364</v>
       </c>
       <c r="D76" s="87"/>
       <c r="E76" s="86" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="F76" s="86" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="G76" s="87"/>
       <c r="H76" s="86" t="s">
@@ -9948,7 +9933,7 @@
       </c>
       <c r="I76" s="87"/>
       <c r="J76" s="89"/>
-      <c r="K76" s="115">
+      <c r="K76" s="116">
         <v>5.0</v>
       </c>
       <c r="L76" s="98" t="s">
@@ -9959,17 +9944,17 @@
     </row>
     <row r="77">
       <c r="A77" s="15" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
       <c r="B77" s="77" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C77" s="99" t="s">
         <v>360</v>
       </c>
       <c r="D77" s="22"/>
       <c r="E77" s="4" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
       <c r="F77" s="22"/>
       <c r="G77" s="22"/>
@@ -9978,7 +9963,7 @@
       </c>
       <c r="I77" s="22"/>
       <c r="J77" s="18"/>
-      <c r="K77" s="116">
+      <c r="K77" s="117">
         <v>5.0</v>
       </c>
       <c r="L77" s="103" t="s">
@@ -9989,20 +9974,20 @@
     </row>
     <row r="78">
       <c r="A78" s="15" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="B78" s="77" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
       <c r="C78" s="99" t="s">
         <v>364</v>
       </c>
       <c r="D78" s="22"/>
       <c r="E78" s="4" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="G78" s="22"/>
       <c r="H78" s="4" t="s">
@@ -10010,28 +9995,28 @@
       </c>
       <c r="I78" s="22"/>
       <c r="J78" s="18"/>
-      <c r="K78" s="116" t="s">
-        <v>640</v>
+      <c r="K78" s="117" t="s">
+        <v>634</v>
       </c>
       <c r="L78" s="4" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="M78" s="4"/>
       <c r="N78" s="18"/>
     </row>
     <row r="79">
       <c r="A79" s="82" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="B79" s="83" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
       <c r="C79" s="84" t="s">
         <v>360</v>
       </c>
       <c r="D79" s="87"/>
       <c r="E79" s="86" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
       <c r="F79" s="87"/>
       <c r="G79" s="87"/>
@@ -10040,7 +10025,7 @@
       </c>
       <c r="I79" s="87"/>
       <c r="J79" s="89"/>
-      <c r="K79" s="115">
+      <c r="K79" s="116">
         <v>5.0</v>
       </c>
       <c r="L79" s="98" t="s">
@@ -10051,20 +10036,20 @@
     </row>
     <row r="80">
       <c r="A80" s="82" t="s">
-        <v>645</v>
+        <v>639</v>
       </c>
       <c r="B80" s="83" t="s">
-        <v>646</v>
+        <v>640</v>
       </c>
       <c r="C80" s="84" t="s">
         <v>364</v>
       </c>
       <c r="D80" s="87"/>
       <c r="E80" s="86" t="s">
-        <v>647</v>
+        <v>641</v>
       </c>
       <c r="F80" s="86" t="s">
-        <v>648</v>
+        <v>642</v>
       </c>
       <c r="G80" s="87"/>
       <c r="H80" s="86" t="s">
@@ -10072,28 +10057,28 @@
       </c>
       <c r="I80" s="87"/>
       <c r="J80" s="89"/>
-      <c r="K80" s="115" t="s">
-        <v>649</v>
+      <c r="K80" s="116" t="s">
+        <v>643</v>
       </c>
       <c r="L80" s="86" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="M80" s="86"/>
       <c r="N80" s="89"/>
     </row>
     <row r="81">
       <c r="A81" s="15" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
       <c r="B81" s="77" t="s">
-        <v>651</v>
+        <v>645</v>
       </c>
       <c r="C81" s="99" t="s">
         <v>360</v>
       </c>
       <c r="D81" s="22"/>
       <c r="E81" s="4" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
       <c r="F81" s="22"/>
       <c r="G81" s="22"/>
@@ -10102,7 +10087,7 @@
       </c>
       <c r="I81" s="22"/>
       <c r="J81" s="18"/>
-      <c r="K81" s="116">
+      <c r="K81" s="117">
         <v>5.0</v>
       </c>
       <c r="L81" s="103" t="s">
@@ -10113,20 +10098,20 @@
     </row>
     <row r="82">
       <c r="A82" s="15" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="B82" s="77" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
       <c r="C82" s="99" t="s">
         <v>364</v>
       </c>
       <c r="D82" s="22"/>
       <c r="E82" s="4" t="s">
-        <v>655</v>
+        <v>649</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>656</v>
+        <v>650</v>
       </c>
       <c r="G82" s="22"/>
       <c r="H82" s="4" t="s">
@@ -10134,7 +10119,7 @@
       </c>
       <c r="I82" s="22"/>
       <c r="J82" s="18"/>
-      <c r="K82" s="116">
+      <c r="K82" s="117">
         <v>5.0</v>
       </c>
       <c r="L82" s="103" t="s">
@@ -10145,17 +10130,17 @@
     </row>
     <row r="83">
       <c r="A83" s="82" t="s">
-        <v>657</v>
+        <v>651</v>
       </c>
       <c r="B83" s="83" t="s">
-        <v>658</v>
+        <v>652</v>
       </c>
       <c r="C83" s="84" t="s">
         <v>360</v>
       </c>
       <c r="D83" s="87"/>
       <c r="E83" s="86" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
       <c r="F83" s="87"/>
       <c r="G83" s="87"/>
@@ -10164,7 +10149,7 @@
       </c>
       <c r="I83" s="87"/>
       <c r="J83" s="89"/>
-      <c r="K83" s="115">
+      <c r="K83" s="116">
         <v>5.0</v>
       </c>
       <c r="L83" s="98" t="s">
@@ -10175,20 +10160,20 @@
     </row>
     <row r="84">
       <c r="A84" s="82" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
       <c r="B84" s="83" t="s">
-        <v>661</v>
+        <v>655</v>
       </c>
       <c r="C84" s="84" t="s">
         <v>364</v>
       </c>
       <c r="D84" s="87"/>
       <c r="E84" s="86" t="s">
-        <v>662</v>
+        <v>656</v>
       </c>
       <c r="F84" s="86" t="s">
-        <v>663</v>
+        <v>657</v>
       </c>
       <c r="G84" s="87"/>
       <c r="H84" s="86" t="s">
@@ -10197,27 +10182,27 @@
       <c r="I84" s="87"/>
       <c r="J84" s="89"/>
       <c r="K84" s="86" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="L84" s="86" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="M84" s="86"/>
       <c r="N84" s="89"/>
     </row>
     <row r="85">
       <c r="A85" s="15" t="s">
-        <v>664</v>
+        <v>658</v>
       </c>
       <c r="B85" s="77" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
       <c r="C85" s="99" t="s">
         <v>360</v>
       </c>
       <c r="D85" s="22"/>
       <c r="E85" s="4" t="s">
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="F85" s="22"/>
       <c r="G85" s="22"/>
@@ -10226,7 +10211,7 @@
       </c>
       <c r="I85" s="22"/>
       <c r="J85" s="18"/>
-      <c r="K85" s="116">
+      <c r="K85" s="117">
         <v>5.0</v>
       </c>
       <c r="L85" s="4" t="s">
@@ -10237,20 +10222,20 @@
     </row>
     <row r="86">
       <c r="A86" s="15" t="s">
-        <v>667</v>
+        <v>661</v>
       </c>
       <c r="B86" s="77" t="s">
-        <v>668</v>
+        <v>662</v>
       </c>
       <c r="C86" s="99" t="s">
         <v>364</v>
       </c>
       <c r="D86" s="22"/>
       <c r="E86" s="4" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>670</v>
+        <v>664</v>
       </c>
       <c r="G86" s="22"/>
       <c r="H86" s="4" t="s">
@@ -10259,153 +10244,153 @@
       <c r="I86" s="22"/>
       <c r="J86" s="18"/>
       <c r="K86" s="4" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="L86" s="4" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="M86" s="4"/>
       <c r="N86" s="18"/>
     </row>
     <row r="87">
-      <c r="A87" s="117" t="s">
-        <v>671</v>
-      </c>
-      <c r="B87" s="118" t="s">
-        <v>672</v>
-      </c>
-      <c r="C87" s="119" t="s">
+      <c r="A87" s="118" t="s">
+        <v>665</v>
+      </c>
+      <c r="B87" s="119" t="s">
+        <v>666</v>
+      </c>
+      <c r="C87" s="120" t="s">
         <v>360</v>
       </c>
-      <c r="D87" s="120"/>
-      <c r="E87" s="121" t="s">
-        <v>673</v>
-      </c>
-      <c r="F87" s="120"/>
-      <c r="G87" s="120"/>
+      <c r="D87" s="121"/>
+      <c r="E87" s="122" t="s">
+        <v>667</v>
+      </c>
+      <c r="F87" s="121"/>
+      <c r="G87" s="121"/>
       <c r="H87" s="109" t="s">
         <v>232</v>
       </c>
-      <c r="I87" s="120"/>
-      <c r="J87" s="122"/>
-      <c r="K87" s="123">
+      <c r="I87" s="121"/>
+      <c r="J87" s="123"/>
+      <c r="K87" s="124">
         <v>5.0</v>
       </c>
-      <c r="L87" s="121" t="s">
+      <c r="L87" s="122" t="s">
         <v>155</v>
       </c>
-      <c r="M87" s="121"/>
-      <c r="N87" s="122"/>
+      <c r="M87" s="122"/>
+      <c r="N87" s="123"/>
     </row>
     <row r="88">
-      <c r="A88" s="117" t="s">
+      <c r="A88" s="118" t="s">
+        <v>668</v>
+      </c>
+      <c r="B88" s="119" t="s">
+        <v>669</v>
+      </c>
+      <c r="C88" s="120" t="s">
+        <v>364</v>
+      </c>
+      <c r="D88" s="121"/>
+      <c r="E88" s="122" t="s">
+        <v>670</v>
+      </c>
+      <c r="F88" s="122" t="s">
+        <v>671</v>
+      </c>
+      <c r="G88" s="125"/>
+      <c r="H88" s="122" t="s">
+        <v>224</v>
+      </c>
+      <c r="I88" s="121"/>
+      <c r="J88" s="123"/>
+      <c r="K88" s="124">
+        <v>5.0</v>
+      </c>
+      <c r="L88" s="122" t="s">
+        <v>155</v>
+      </c>
+      <c r="M88" s="122"/>
+      <c r="N88" s="123"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="118" t="s">
+        <v>672</v>
+      </c>
+      <c r="B89" s="119" t="s">
+        <v>673</v>
+      </c>
+      <c r="C89" s="120" t="s">
+        <v>364</v>
+      </c>
+      <c r="D89" s="121"/>
+      <c r="E89" s="122" t="s">
+        <v>670</v>
+      </c>
+      <c r="F89" s="122" t="s">
         <v>674</v>
       </c>
-      <c r="B88" s="118" t="s">
+      <c r="G89" s="121"/>
+      <c r="H89" s="122" t="s">
+        <v>232</v>
+      </c>
+      <c r="I89" s="121"/>
+      <c r="J89" s="123"/>
+      <c r="K89" s="124" t="s">
         <v>675</v>
       </c>
-      <c r="C88" s="119" t="s">
+      <c r="L89" s="122" t="s">
+        <v>676</v>
+      </c>
+      <c r="M89" s="122"/>
+      <c r="N89" s="123"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="118" t="s">
+        <v>677</v>
+      </c>
+      <c r="B90" s="119" t="s">
+        <v>678</v>
+      </c>
+      <c r="C90" s="120" t="s">
         <v>364</v>
       </c>
-      <c r="D88" s="120"/>
-      <c r="E88" s="121" t="s">
-        <v>676</v>
-      </c>
-      <c r="F88" s="121" t="s">
-        <v>677</v>
-      </c>
-      <c r="G88" s="124"/>
-      <c r="H88" s="121" t="s">
-        <v>224</v>
-      </c>
-      <c r="I88" s="120"/>
-      <c r="J88" s="122"/>
-      <c r="K88" s="123">
-        <v>5.0</v>
-      </c>
-      <c r="L88" s="121" t="s">
-        <v>155</v>
-      </c>
-      <c r="M88" s="121"/>
-      <c r="N88" s="122"/>
-    </row>
-    <row r="89">
-      <c r="A89" s="117" t="s">
-        <v>678</v>
-      </c>
-      <c r="B89" s="118" t="s">
+      <c r="D90" s="121"/>
+      <c r="E90" s="122" t="s">
+        <v>670</v>
+      </c>
+      <c r="F90" s="122" t="s">
         <v>679</v>
       </c>
-      <c r="C89" s="119" t="s">
-        <v>364</v>
-      </c>
-      <c r="D89" s="120"/>
-      <c r="E89" s="121" t="s">
-        <v>676</v>
-      </c>
-      <c r="F89" s="121" t="s">
+      <c r="G90" s="121"/>
+      <c r="H90" s="122" t="s">
+        <v>232</v>
+      </c>
+      <c r="I90" s="121"/>
+      <c r="J90" s="123"/>
+      <c r="K90" s="124" t="s">
         <v>680</v>
       </c>
-      <c r="G89" s="120"/>
-      <c r="H89" s="121" t="s">
-        <v>232</v>
-      </c>
-      <c r="I89" s="120"/>
-      <c r="J89" s="122"/>
-      <c r="K89" s="123" t="s">
+      <c r="L90" s="122" t="s">
         <v>681</v>
       </c>
-      <c r="L89" s="121" t="s">
-        <v>682</v>
-      </c>
-      <c r="M89" s="121"/>
-      <c r="N89" s="122"/>
-    </row>
-    <row r="90">
-      <c r="A90" s="117" t="s">
-        <v>683</v>
-      </c>
-      <c r="B90" s="118" t="s">
-        <v>684</v>
-      </c>
-      <c r="C90" s="119" t="s">
-        <v>364</v>
-      </c>
-      <c r="D90" s="120"/>
-      <c r="E90" s="121" t="s">
-        <v>676</v>
-      </c>
-      <c r="F90" s="121" t="s">
-        <v>685</v>
-      </c>
-      <c r="G90" s="120"/>
-      <c r="H90" s="121" t="s">
-        <v>232</v>
-      </c>
-      <c r="I90" s="120"/>
-      <c r="J90" s="122"/>
-      <c r="K90" s="123" t="s">
-        <v>686</v>
-      </c>
-      <c r="L90" s="121" t="s">
-        <v>687</v>
-      </c>
-      <c r="M90" s="121"/>
-      <c r="N90" s="122"/>
+      <c r="M90" s="122"/>
+      <c r="N90" s="123"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="82" t="s">
-        <v>688</v>
+        <v>682</v>
       </c>
       <c r="B91" s="83" t="s">
-        <v>689</v>
+        <v>683</v>
       </c>
       <c r="C91" s="84" t="s">
         <v>360</v>
       </c>
       <c r="D91" s="87"/>
       <c r="E91" s="86" t="s">
-        <v>690</v>
+        <v>684</v>
       </c>
       <c r="F91" s="87"/>
       <c r="G91" s="87"/>
@@ -10414,7 +10399,7 @@
       </c>
       <c r="I91" s="87"/>
       <c r="J91" s="89"/>
-      <c r="K91" s="115">
+      <c r="K91" s="116">
         <v>3.0</v>
       </c>
       <c r="L91" s="86" t="s">
@@ -10425,20 +10410,20 @@
     </row>
     <row r="92">
       <c r="A92" s="82" t="s">
-        <v>691</v>
+        <v>685</v>
       </c>
       <c r="B92" s="83" t="s">
-        <v>692</v>
+        <v>686</v>
       </c>
       <c r="C92" s="84" t="s">
         <v>364</v>
       </c>
       <c r="D92" s="87"/>
       <c r="E92" s="86" t="s">
-        <v>693</v>
+        <v>687</v>
       </c>
       <c r="F92" s="86" t="s">
-        <v>694</v>
+        <v>688</v>
       </c>
       <c r="G92" s="87"/>
       <c r="H92" s="86" t="s">
@@ -10446,31 +10431,31 @@
       </c>
       <c r="I92" s="87"/>
       <c r="J92" s="89"/>
-      <c r="K92" s="115" t="s">
-        <v>695</v>
+      <c r="K92" s="116" t="s">
+        <v>689</v>
       </c>
       <c r="L92" s="86" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="M92" s="86"/>
       <c r="N92" s="89"/>
     </row>
     <row r="93">
       <c r="A93" s="82" t="s">
-        <v>696</v>
+        <v>690</v>
       </c>
       <c r="B93" s="83" t="s">
-        <v>697</v>
+        <v>691</v>
       </c>
       <c r="C93" s="84" t="s">
         <v>364</v>
       </c>
       <c r="D93" s="87"/>
       <c r="E93" s="86" t="s">
-        <v>693</v>
+        <v>687</v>
       </c>
       <c r="F93" s="86" t="s">
-        <v>698</v>
+        <v>692</v>
       </c>
       <c r="G93" s="87"/>
       <c r="H93" s="86" t="s">
@@ -10478,7 +10463,7 @@
       </c>
       <c r="I93" s="87"/>
       <c r="J93" s="89"/>
-      <c r="K93" s="125">
+      <c r="K93" s="126">
         <v>3.0</v>
       </c>
       <c r="L93" s="86" t="s">
@@ -10489,20 +10474,20 @@
     </row>
     <row r="94">
       <c r="A94" s="82" t="s">
-        <v>699</v>
+        <v>693</v>
       </c>
       <c r="B94" s="83" t="s">
-        <v>700</v>
+        <v>694</v>
       </c>
       <c r="C94" s="84" t="s">
         <v>364</v>
       </c>
       <c r="D94" s="87"/>
       <c r="E94" s="86" t="s">
-        <v>693</v>
+        <v>687</v>
       </c>
       <c r="F94" s="86" t="s">
-        <v>701</v>
+        <v>695</v>
       </c>
       <c r="G94" s="87"/>
       <c r="H94" s="86" t="s">
@@ -10510,28 +10495,28 @@
       </c>
       <c r="I94" s="87"/>
       <c r="J94" s="89"/>
-      <c r="K94" s="115" t="s">
-        <v>702</v>
+      <c r="K94" s="116" t="s">
+        <v>696</v>
       </c>
       <c r="L94" s="86" t="s">
-        <v>682</v>
+        <v>676</v>
       </c>
       <c r="M94" s="86"/>
       <c r="N94" s="89"/>
     </row>
     <row r="95">
       <c r="A95" s="15" t="s">
-        <v>703</v>
+        <v>697</v>
       </c>
       <c r="B95" s="77" t="s">
-        <v>704</v>
+        <v>698</v>
       </c>
       <c r="C95" s="99" t="s">
         <v>360</v>
       </c>
       <c r="D95" s="22"/>
       <c r="E95" s="4" t="s">
-        <v>705</v>
+        <v>699</v>
       </c>
       <c r="F95" s="22"/>
       <c r="G95" s="22"/>
@@ -10540,7 +10525,7 @@
       </c>
       <c r="I95" s="22"/>
       <c r="J95" s="18"/>
-      <c r="K95" s="116">
+      <c r="K95" s="117">
         <v>3.0</v>
       </c>
       <c r="L95" s="4" t="s">
@@ -10551,20 +10536,20 @@
     </row>
     <row r="96">
       <c r="A96" s="15" t="s">
-        <v>706</v>
+        <v>700</v>
       </c>
       <c r="B96" s="77" t="s">
-        <v>707</v>
+        <v>701</v>
       </c>
       <c r="C96" s="99" t="s">
         <v>364</v>
       </c>
       <c r="D96" s="22"/>
       <c r="E96" s="4" t="s">
-        <v>708</v>
+        <v>702</v>
       </c>
       <c r="F96" s="4" t="s">
-        <v>709</v>
+        <v>703</v>
       </c>
       <c r="G96" s="22"/>
       <c r="H96" s="4" t="s">
@@ -10572,28 +10557,28 @@
       </c>
       <c r="I96" s="22"/>
       <c r="J96" s="18"/>
-      <c r="K96" s="116" t="s">
-        <v>710</v>
+      <c r="K96" s="117" t="s">
+        <v>704</v>
       </c>
       <c r="L96" s="4" t="s">
-        <v>711</v>
+        <v>705</v>
       </c>
       <c r="M96" s="4"/>
       <c r="N96" s="18"/>
     </row>
     <row r="97">
       <c r="A97" s="82" t="s">
-        <v>712</v>
+        <v>706</v>
       </c>
       <c r="B97" s="83" t="s">
-        <v>713</v>
+        <v>707</v>
       </c>
       <c r="C97" s="84" t="s">
         <v>360</v>
       </c>
       <c r="D97" s="87"/>
       <c r="E97" s="86" t="s">
-        <v>714</v>
+        <v>708</v>
       </c>
       <c r="F97" s="87"/>
       <c r="G97" s="87"/>
@@ -10602,7 +10587,7 @@
       </c>
       <c r="I97" s="87"/>
       <c r="J97" s="89"/>
-      <c r="K97" s="115">
+      <c r="K97" s="116">
         <v>3.0</v>
       </c>
       <c r="L97" s="86" t="s">
@@ -10613,20 +10598,20 @@
     </row>
     <row r="98">
       <c r="A98" s="82" t="s">
-        <v>715</v>
+        <v>709</v>
       </c>
       <c r="B98" s="83" t="s">
-        <v>716</v>
+        <v>710</v>
       </c>
       <c r="C98" s="84" t="s">
         <v>364</v>
       </c>
       <c r="D98" s="87"/>
       <c r="E98" s="86" t="s">
-        <v>717</v>
+        <v>711</v>
       </c>
       <c r="F98" s="86" t="s">
-        <v>718</v>
+        <v>712</v>
       </c>
       <c r="G98" s="87"/>
       <c r="H98" s="86" t="s">
@@ -10634,28 +10619,28 @@
       </c>
       <c r="I98" s="87"/>
       <c r="J98" s="89"/>
-      <c r="K98" s="115" t="s">
-        <v>695</v>
+      <c r="K98" s="116" t="s">
+        <v>689</v>
       </c>
       <c r="L98" s="86" t="s">
-        <v>719</v>
+        <v>713</v>
       </c>
       <c r="M98" s="86"/>
       <c r="N98" s="89"/>
     </row>
     <row r="99">
       <c r="A99" s="15" t="s">
-        <v>720</v>
+        <v>714</v>
       </c>
       <c r="B99" s="77" t="s">
-        <v>721</v>
+        <v>715</v>
       </c>
       <c r="C99" s="99" t="s">
         <v>360</v>
       </c>
       <c r="D99" s="22"/>
       <c r="E99" s="4" t="s">
-        <v>722</v>
+        <v>716</v>
       </c>
       <c r="F99" s="22"/>
       <c r="G99" s="22"/>
@@ -10664,7 +10649,7 @@
       </c>
       <c r="I99" s="22"/>
       <c r="J99" s="18"/>
-      <c r="K99" s="116">
+      <c r="K99" s="117">
         <v>5.0</v>
       </c>
       <c r="L99" s="4" t="s">
@@ -10675,20 +10660,20 @@
     </row>
     <row r="100">
       <c r="A100" s="58" t="s">
-        <v>723</v>
+        <v>717</v>
       </c>
       <c r="B100" s="77" t="s">
-        <v>724</v>
+        <v>718</v>
       </c>
       <c r="C100" s="99" t="s">
         <v>364</v>
       </c>
       <c r="D100" s="22"/>
       <c r="E100" s="4" t="s">
-        <v>725</v>
+        <v>719</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>726</v>
+        <v>720</v>
       </c>
       <c r="G100" s="22"/>
       <c r="H100" s="4" t="s">
@@ -10697,27 +10682,27 @@
       <c r="I100" s="22"/>
       <c r="J100" s="18"/>
       <c r="K100" s="4" t="s">
-        <v>727</v>
+        <v>721</v>
       </c>
       <c r="L100" s="4" t="s">
-        <v>728</v>
+        <v>722</v>
       </c>
       <c r="M100" s="4"/>
       <c r="N100" s="18"/>
     </row>
     <row r="101">
       <c r="A101" s="15" t="s">
-        <v>729</v>
+        <v>723</v>
       </c>
       <c r="B101" s="77" t="s">
-        <v>730</v>
+        <v>724</v>
       </c>
       <c r="C101" s="99" t="s">
         <v>360</v>
       </c>
       <c r="D101" s="22"/>
       <c r="E101" s="4" t="s">
-        <v>731</v>
+        <v>725</v>
       </c>
       <c r="F101" s="22"/>
       <c r="G101" s="22"/>
@@ -10726,7 +10711,7 @@
       </c>
       <c r="I101" s="22"/>
       <c r="J101" s="18"/>
-      <c r="K101" s="116">
+      <c r="K101" s="117">
         <v>5.0</v>
       </c>
       <c r="L101" s="4" t="s">
@@ -10737,20 +10722,20 @@
     </row>
     <row r="102">
       <c r="A102" s="58" t="s">
-        <v>732</v>
+        <v>726</v>
       </c>
       <c r="B102" s="77" t="s">
-        <v>733</v>
+        <v>727</v>
       </c>
       <c r="C102" s="99" t="s">
         <v>364</v>
       </c>
       <c r="D102" s="22"/>
       <c r="E102" s="4" t="s">
-        <v>734</v>
+        <v>728</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>735</v>
+        <v>729</v>
       </c>
       <c r="G102" s="22"/>
       <c r="H102" s="4" t="s">
@@ -10759,10 +10744,10 @@
       <c r="I102" s="22"/>
       <c r="J102" s="18"/>
       <c r="K102" s="4" t="s">
-        <v>727</v>
+        <v>721</v>
       </c>
       <c r="L102" s="4" t="s">
-        <v>728</v>
+        <v>722</v>
       </c>
       <c r="M102" s="4"/>
       <c r="N102" s="18"/>
@@ -10794,555 +10779,555 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="127" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="127" t="s">
+      <c r="B1" s="128" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="127" t="s">
-        <v>736</v>
-      </c>
-      <c r="D1" s="126" t="s">
+      <c r="C1" s="128" t="s">
+        <v>730</v>
+      </c>
+      <c r="D1" s="127" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="126" t="s">
+      <c r="E1" s="127" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="128" t="s">
-        <v>737</v>
+      <c r="A2" s="129" t="s">
+        <v>731</v>
       </c>
       <c r="B2" s="62" t="s">
-        <v>738</v>
+        <v>732</v>
       </c>
       <c r="C2" s="62"/>
       <c r="D2" s="62" t="s">
-        <v>739</v>
+        <v>733</v>
       </c>
       <c r="E2" s="18"/>
     </row>
     <row r="3">
-      <c r="A3" s="128" t="s">
-        <v>740</v>
+      <c r="A3" s="129" t="s">
+        <v>734</v>
       </c>
       <c r="B3" s="62" t="s">
-        <v>741</v>
+        <v>735</v>
       </c>
       <c r="C3" s="62"/>
       <c r="D3" s="62" t="s">
-        <v>742</v>
+        <v>736</v>
       </c>
       <c r="E3" s="18"/>
     </row>
     <row r="4">
-      <c r="A4" s="128" t="s">
-        <v>743</v>
+      <c r="A4" s="129" t="s">
+        <v>737</v>
       </c>
       <c r="B4" s="62" t="s">
-        <v>744</v>
+        <v>738</v>
       </c>
       <c r="C4" s="62"/>
       <c r="D4" s="18" t="s">
-        <v>745</v>
+        <v>739</v>
       </c>
       <c r="E4" s="62"/>
     </row>
     <row r="5">
-      <c r="A5" s="128" t="s">
-        <v>746</v>
+      <c r="A5" s="129" t="s">
+        <v>740</v>
       </c>
       <c r="B5" s="62" t="s">
-        <v>747</v>
+        <v>741</v>
       </c>
       <c r="C5" s="62"/>
       <c r="D5" s="18" t="s">
+        <v>742</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="129" t="s">
+        <v>743</v>
+      </c>
+      <c r="B6" s="130" t="s">
+        <v>744</v>
+      </c>
+      <c r="C6" s="130"/>
+      <c r="D6" s="18" t="s">
+        <v>745</v>
+      </c>
+      <c r="E6" s="131" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="129" t="s">
+        <v>747</v>
+      </c>
+      <c r="B7" s="62" t="s">
         <v>748</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="128" t="s">
-        <v>749</v>
-      </c>
-      <c r="B6" s="129" t="s">
-        <v>750</v>
-      </c>
-      <c r="C6" s="129"/>
-      <c r="D6" s="18" t="s">
-        <v>751</v>
-      </c>
-      <c r="E6" s="130" t="s">
-        <v>752</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="128" t="s">
-        <v>753</v>
-      </c>
-      <c r="B7" s="62" t="s">
-        <v>754</v>
       </c>
       <c r="C7" s="62"/>
       <c r="D7" s="18" t="s">
-        <v>755</v>
+        <v>749</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>749</v>
+        <v>743</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="128" t="s">
-        <v>756</v>
+      <c r="A8" s="129" t="s">
+        <v>750</v>
       </c>
       <c r="B8" s="62" t="s">
-        <v>757</v>
+        <v>751</v>
       </c>
       <c r="C8" s="62"/>
       <c r="D8" s="62" t="s">
-        <v>758</v>
+        <v>752</v>
       </c>
       <c r="E8" s="18"/>
     </row>
     <row r="9">
-      <c r="A9" s="128" t="s">
-        <v>759</v>
+      <c r="A9" s="129" t="s">
+        <v>753</v>
       </c>
       <c r="B9" s="62" t="s">
-        <v>760</v>
+        <v>754</v>
       </c>
       <c r="C9" s="62"/>
       <c r="D9" s="62" t="s">
+        <v>755</v>
+      </c>
+      <c r="E9" s="18"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="129" t="s">
+        <v>756</v>
+      </c>
+      <c r="B10" s="62" t="s">
+        <v>757</v>
+      </c>
+      <c r="C10" s="62"/>
+      <c r="D10" s="132" t="s">
+        <v>758</v>
+      </c>
+      <c r="E10" s="18"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="129" t="s">
+        <v>759</v>
+      </c>
+      <c r="B11" s="62" t="s">
+        <v>760</v>
+      </c>
+      <c r="C11" s="62"/>
+      <c r="D11" s="132" t="s">
         <v>761</v>
       </c>
-      <c r="E9" s="18"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="128" t="s">
+      <c r="E11" s="18"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="129" t="s">
         <v>762</v>
       </c>
-      <c r="B10" s="62" t="s">
+      <c r="B12" s="62" t="s">
         <v>763</v>
       </c>
-      <c r="C10" s="62"/>
-      <c r="D10" s="131" t="s">
+      <c r="C12" s="62"/>
+      <c r="D12" s="132" t="s">
         <v>764</v>
       </c>
-      <c r="E10" s="18"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="128" t="s">
+      <c r="E12" s="18"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="129" t="s">
         <v>765</v>
       </c>
-      <c r="B11" s="62" t="s">
+      <c r="B13" s="62" t="s">
         <v>766</v>
       </c>
-      <c r="C11" s="62"/>
-      <c r="D11" s="131" t="s">
+      <c r="C13" s="62"/>
+      <c r="D13" s="132" t="s">
         <v>767</v>
       </c>
-      <c r="E11" s="18"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="128" t="s">
+      <c r="E13" s="18"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="129" t="s">
         <v>768</v>
       </c>
-      <c r="B12" s="62" t="s">
+      <c r="B14" s="62" t="s">
         <v>769</v>
       </c>
-      <c r="C12" s="62"/>
-      <c r="D12" s="131" t="s">
+      <c r="C14" s="62"/>
+      <c r="D14" s="132" t="s">
         <v>770</v>
       </c>
-      <c r="E12" s="18"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="128" t="s">
+      <c r="E14" s="18"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="129" t="s">
         <v>771</v>
       </c>
-      <c r="B13" s="62" t="s">
+      <c r="B15" s="62" t="s">
         <v>772</v>
       </c>
-      <c r="C13" s="62"/>
-      <c r="D13" s="131" t="s">
+      <c r="C15" s="62"/>
+      <c r="D15" s="132" t="s">
         <v>773</v>
       </c>
-      <c r="E13" s="18"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="128" t="s">
+      <c r="E15" s="18"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="129" t="s">
         <v>774</v>
       </c>
-      <c r="B14" s="62" t="s">
+      <c r="B16" s="62" t="s">
         <v>775</v>
       </c>
-      <c r="C14" s="62"/>
-      <c r="D14" s="131" t="s">
+      <c r="C16" s="62"/>
+      <c r="D16" s="132" t="s">
         <v>776</v>
       </c>
-      <c r="E14" s="18"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="128" t="s">
+      <c r="E16" s="18"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="129" t="s">
         <v>777</v>
       </c>
-      <c r="B15" s="62" t="s">
+      <c r="B17" s="133" t="s">
+        <v>744</v>
+      </c>
+      <c r="C17" s="133"/>
+      <c r="D17" s="132" t="s">
         <v>778</v>
       </c>
-      <c r="C15" s="62"/>
-      <c r="D15" s="131" t="s">
+      <c r="E17" s="18"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="129" t="s">
         <v>779</v>
       </c>
-      <c r="E15" s="18"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="128" t="s">
+      <c r="B18" s="29" t="s">
         <v>780</v>
-      </c>
-      <c r="B16" s="62" t="s">
-        <v>781</v>
-      </c>
-      <c r="C16" s="62"/>
-      <c r="D16" s="131" t="s">
-        <v>782</v>
-      </c>
-      <c r="E16" s="18"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="128" t="s">
-        <v>783</v>
-      </c>
-      <c r="B17" s="132" t="s">
-        <v>750</v>
-      </c>
-      <c r="C17" s="132"/>
-      <c r="D17" s="131" t="s">
-        <v>784</v>
-      </c>
-      <c r="E17" s="18"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="128" t="s">
-        <v>785</v>
-      </c>
-      <c r="B18" s="29" t="s">
-        <v>786</v>
       </c>
       <c r="C18" s="29"/>
       <c r="D18" s="62" t="s">
+        <v>781</v>
+      </c>
+      <c r="E18" s="18"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="129" t="s">
+        <v>782</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>783</v>
+      </c>
+      <c r="C19" s="134" t="s">
+        <v>784</v>
+      </c>
+      <c r="D19" s="132" t="s">
+        <v>785</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="129" t="s">
+        <v>786</v>
+      </c>
+      <c r="B20" s="135" t="s">
         <v>787</v>
       </c>
-      <c r="E18" s="18"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="128" t="s">
+      <c r="C20" s="135"/>
+      <c r="D20" s="18" t="s">
         <v>788</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="E20" s="18"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="129" t="s">
         <v>789</v>
       </c>
-      <c r="C19" s="133" t="s">
+      <c r="B21" s="135" t="s">
         <v>790</v>
       </c>
-      <c r="D19" s="131" t="s">
+      <c r="C21" s="135"/>
+      <c r="D21" s="18" t="s">
         <v>791</v>
       </c>
-      <c r="E19" s="20" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="128" t="s">
+      <c r="E21" s="18"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="129" t="s">
         <v>792</v>
       </c>
-      <c r="B20" s="134" t="s">
+      <c r="B22" s="16" t="s">
+        <v>783</v>
+      </c>
+      <c r="C22" s="135" t="s">
         <v>793</v>
       </c>
-      <c r="C20" s="134"/>
-      <c r="D20" s="18" t="s">
+      <c r="D22" s="18" t="s">
         <v>794</v>
       </c>
-      <c r="E20" s="18"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="128" t="s">
+      <c r="E22" s="20" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="129" t="s">
         <v>795</v>
       </c>
-      <c r="B21" s="134" t="s">
+      <c r="B23" s="62" t="s">
         <v>796</v>
-      </c>
-      <c r="C21" s="134"/>
-      <c r="D21" s="18" t="s">
-        <v>797</v>
-      </c>
-      <c r="E21" s="18"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="128" t="s">
-        <v>798</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>789</v>
-      </c>
-      <c r="C22" s="134" t="s">
-        <v>799</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>800</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="128" t="s">
-        <v>801</v>
-      </c>
-      <c r="B23" s="62" t="s">
-        <v>802</v>
       </c>
       <c r="C23" s="62"/>
       <c r="D23" s="62" t="s">
-        <v>803</v>
+        <v>797</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>759</v>
+        <v>753</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="128" t="s">
-        <v>804</v>
-      </c>
-      <c r="B24" s="135" t="s">
-        <v>805</v>
-      </c>
-      <c r="C24" s="135"/>
+      <c r="A24" s="129" t="s">
+        <v>798</v>
+      </c>
+      <c r="B24" s="136" t="s">
+        <v>799</v>
+      </c>
+      <c r="C24" s="136"/>
       <c r="D24" s="20" t="s">
-        <v>806</v>
+        <v>800</v>
       </c>
       <c r="E24" s="18"/>
     </row>
     <row r="25">
-      <c r="A25" s="128" t="s">
-        <v>807</v>
+      <c r="A25" s="129" t="s">
+        <v>801</v>
       </c>
       <c r="B25" s="62" t="s">
-        <v>808</v>
+        <v>802</v>
       </c>
       <c r="C25" s="62"/>
       <c r="D25" s="62" t="s">
-        <v>809</v>
+        <v>803</v>
       </c>
       <c r="E25" s="18"/>
     </row>
     <row r="26">
-      <c r="A26" s="136" t="s">
-        <v>810</v>
+      <c r="A26" s="137" t="s">
+        <v>804</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>811</v>
+        <v>805</v>
       </c>
       <c r="C26" s="29"/>
       <c r="D26" s="29" t="s">
-        <v>812</v>
+        <v>806</v>
       </c>
       <c r="E26" s="28"/>
     </row>
     <row r="27">
-      <c r="A27" s="136" t="s">
-        <v>813</v>
+      <c r="A27" s="137" t="s">
+        <v>807</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>814</v>
+        <v>808</v>
       </c>
       <c r="C27" s="29"/>
       <c r="D27" s="29" t="s">
-        <v>815</v>
+        <v>809</v>
       </c>
       <c r="E27" s="28"/>
     </row>
     <row r="28">
-      <c r="A28" s="136" t="s">
-        <v>816</v>
+      <c r="A28" s="137" t="s">
+        <v>810</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>817</v>
+        <v>811</v>
       </c>
       <c r="C28" s="29"/>
       <c r="D28" s="29" t="s">
-        <v>818</v>
+        <v>812</v>
       </c>
       <c r="E28" s="28"/>
     </row>
     <row r="29">
-      <c r="A29" s="136" t="s">
-        <v>819</v>
+      <c r="A29" s="137" t="s">
+        <v>813</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="C29" s="29"/>
       <c r="D29" s="29" t="s">
-        <v>821</v>
+        <v>815</v>
       </c>
       <c r="E29" s="28"/>
     </row>
     <row r="30">
-      <c r="A30" s="136" t="s">
-        <v>822</v>
+      <c r="A30" s="137" t="s">
+        <v>816</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>823</v>
+        <v>817</v>
       </c>
       <c r="C30" s="29"/>
       <c r="D30" s="29" t="s">
-        <v>824</v>
+        <v>818</v>
       </c>
       <c r="E30" s="28"/>
     </row>
     <row r="31">
-      <c r="A31" s="136" t="s">
-        <v>825</v>
+      <c r="A31" s="137" t="s">
+        <v>819</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>826</v>
+        <v>820</v>
       </c>
       <c r="C31" s="29"/>
       <c r="D31" s="29" t="s">
-        <v>827</v>
+        <v>821</v>
       </c>
       <c r="E31" s="28"/>
     </row>
     <row r="32">
-      <c r="A32" s="136" t="s">
-        <v>828</v>
+      <c r="A32" s="137" t="s">
+        <v>822</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>829</v>
+        <v>823</v>
       </c>
       <c r="C32" s="29"/>
       <c r="D32" s="29" t="s">
-        <v>830</v>
+        <v>824</v>
       </c>
       <c r="E32" s="28"/>
     </row>
     <row r="33">
-      <c r="A33" s="136" t="s">
-        <v>831</v>
+      <c r="A33" s="137" t="s">
+        <v>825</v>
       </c>
       <c r="B33" s="29" t="s">
-        <v>832</v>
+        <v>826</v>
       </c>
       <c r="C33" s="29"/>
       <c r="D33" s="29" t="s">
-        <v>833</v>
+        <v>827</v>
       </c>
       <c r="E33" s="28"/>
     </row>
     <row r="34">
-      <c r="A34" s="136" t="s">
-        <v>834</v>
+      <c r="A34" s="137" t="s">
+        <v>828</v>
       </c>
       <c r="B34" s="29" t="s">
-        <v>835</v>
+        <v>829</v>
       </c>
       <c r="C34" s="29"/>
       <c r="D34" s="29" t="s">
-        <v>836</v>
+        <v>830</v>
       </c>
       <c r="E34" s="28"/>
     </row>
     <row r="35">
-      <c r="A35" s="136" t="s">
-        <v>837</v>
+      <c r="A35" s="137" t="s">
+        <v>831</v>
       </c>
       <c r="B35" s="29" t="s">
-        <v>838</v>
+        <v>832</v>
       </c>
       <c r="C35" s="29"/>
       <c r="D35" s="29" t="s">
+        <v>833</v>
+      </c>
+      <c r="E35" s="28"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="117" t="s">
+        <v>834</v>
+      </c>
+      <c r="B36" s="138" t="s">
+        <v>835</v>
+      </c>
+      <c r="C36" s="138"/>
+      <c r="D36" s="22" t="s">
+        <v>836</v>
+      </c>
+      <c r="E36" s="18"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="117" t="s">
+        <v>837</v>
+      </c>
+      <c r="B37" s="138" t="s">
+        <v>838</v>
+      </c>
+      <c r="C37" s="138"/>
+      <c r="D37" s="22" t="s">
         <v>839</v>
       </c>
-      <c r="E35" s="28"/>
-    </row>
-    <row r="36">
-      <c r="A36" s="116" t="s">
+      <c r="E37" s="18"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="117" t="s">
         <v>840</v>
       </c>
-      <c r="B36" s="137" t="s">
+      <c r="B38" s="138" t="s">
         <v>841</v>
       </c>
-      <c r="C36" s="137"/>
-      <c r="D36" s="22" t="s">
+      <c r="C38" s="138"/>
+      <c r="D38" s="22" t="s">
         <v>842</v>
       </c>
-      <c r="E36" s="18"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="116" t="s">
+      <c r="E38" s="18"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="117" t="s">
         <v>843</v>
       </c>
-      <c r="B37" s="137" t="s">
+      <c r="B39" s="139" t="s">
         <v>844</v>
       </c>
-      <c r="C37" s="137"/>
-      <c r="D37" s="22" t="s">
+      <c r="C39" s="139"/>
+      <c r="D39" s="22" t="s">
+        <v>736</v>
+      </c>
+      <c r="E39" s="18"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="117" t="s">
         <v>845</v>
       </c>
-      <c r="E37" s="18"/>
-    </row>
-    <row r="38">
-      <c r="A38" s="116" t="s">
+      <c r="B40" s="139" t="s">
         <v>846</v>
       </c>
-      <c r="B38" s="137" t="s">
+      <c r="C40" s="139"/>
+      <c r="D40" s="22" t="s">
         <v>847</v>
       </c>
-      <c r="C38" s="137"/>
-      <c r="D38" s="22" t="s">
+      <c r="E40" s="18"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="117" t="s">
         <v>848</v>
       </c>
-      <c r="E38" s="18"/>
-    </row>
-    <row r="39">
-      <c r="A39" s="116" t="s">
+      <c r="B41" s="140" t="s">
         <v>849</v>
       </c>
-      <c r="B39" s="138" t="s">
+      <c r="C41" s="140"/>
+      <c r="D41" s="22" t="s">
         <v>850</v>
-      </c>
-      <c r="C39" s="138"/>
-      <c r="D39" s="22" t="s">
-        <v>742</v>
-      </c>
-      <c r="E39" s="18"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="116" t="s">
-        <v>851</v>
-      </c>
-      <c r="B40" s="138" t="s">
-        <v>852</v>
-      </c>
-      <c r="C40" s="138"/>
-      <c r="D40" s="22" t="s">
-        <v>853</v>
-      </c>
-      <c r="E40" s="18"/>
-    </row>
-    <row r="41">
-      <c r="A41" s="116" t="s">
-        <v>854</v>
-      </c>
-      <c r="B41" s="139" t="s">
-        <v>855</v>
-      </c>
-      <c r="C41" s="139"/>
-      <c r="D41" s="22" t="s">
-        <v>856</v>
       </c>
       <c r="E41" s="18"/>
     </row>
@@ -11363,16 +11348,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="18" t="s">
-        <v>857</v>
+        <v>851</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>858</v>
+        <v>852</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>859</v>
+        <v>853</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>860</v>
+        <v>854</v>
       </c>
       <c r="E1" s="18"/>
       <c r="F1" s="18"/>
@@ -11387,13 +11372,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>861</v>
+        <v>855</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>862</v>
+        <v>856</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>863</v>
+        <v>857</v>
       </c>
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
@@ -11431,13 +11416,13 @@
     </row>
     <row r="5">
       <c r="A5" s="18" t="s">
-        <v>864</v>
+        <v>858</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>865</v>
+        <v>859</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>866</v>
+        <v>860</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
@@ -11453,10 +11438,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>867</v>
+        <v>861</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>868</v>
+        <v>862</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="18"/>
@@ -11470,10 +11455,10 @@
     <row r="7">
       <c r="A7" s="18"/>
       <c r="B7" s="18" t="s">
-        <v>869</v>
+        <v>863</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>868</v>
+        <v>862</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
@@ -11487,10 +11472,10 @@
     <row r="8">
       <c r="A8" s="18"/>
       <c r="B8" s="18" t="s">
-        <v>870</v>
+        <v>864</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>868</v>
+        <v>862</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
@@ -11504,10 +11489,10 @@
     <row r="9">
       <c r="A9" s="18"/>
       <c r="B9" s="18" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>868</v>
+        <v>862</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
@@ -11533,10 +11518,10 @@
     </row>
     <row r="11">
       <c r="A11" s="18" t="s">
-        <v>872</v>
+        <v>866</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>873</v>
+        <v>867</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
@@ -11550,10 +11535,10 @@
     </row>
     <row r="12">
       <c r="A12" s="18" t="s">
-        <v>874</v>
-      </c>
-      <c r="B12" s="140" t="s">
-        <v>875</v>
+        <v>868</v>
+      </c>
+      <c r="B12" s="141" t="s">
+        <v>869</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
@@ -11567,10 +11552,10 @@
     </row>
     <row r="13">
       <c r="A13" s="18" t="s">
-        <v>876</v>
-      </c>
-      <c r="B13" s="140" t="s">
-        <v>877</v>
+        <v>870</v>
+      </c>
+      <c r="B13" s="141" t="s">
+        <v>871</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
@@ -11584,10 +11569,10 @@
     </row>
     <row r="14">
       <c r="A14" s="18" t="s">
-        <v>878</v>
-      </c>
-      <c r="B14" s="140" t="s">
-        <v>879</v>
+        <v>872</v>
+      </c>
+      <c r="B14" s="141" t="s">
+        <v>873</v>
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
@@ -11601,10 +11586,10 @@
     </row>
     <row r="15">
       <c r="A15" s="18" t="s">
-        <v>880</v>
-      </c>
-      <c r="B15" s="140" t="s">
-        <v>881</v>
+        <v>874</v>
+      </c>
+      <c r="B15" s="141" t="s">
+        <v>875</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
@@ -11618,10 +11603,10 @@
     </row>
     <row r="16">
       <c r="A16" s="18" t="s">
-        <v>882</v>
-      </c>
-      <c r="B16" s="140" t="s">
-        <v>883</v>
+        <v>876</v>
+      </c>
+      <c r="B16" s="141" t="s">
+        <v>877</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
@@ -11635,10 +11620,10 @@
     </row>
     <row r="17">
       <c r="A17" s="18" t="s">
-        <v>884</v>
-      </c>
-      <c r="B17" s="140" t="s">
-        <v>885</v>
+        <v>878</v>
+      </c>
+      <c r="B17" s="141" t="s">
+        <v>879</v>
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
@@ -11652,10 +11637,10 @@
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>886</v>
+        <v>880</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>887</v>
+        <v>881</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
@@ -11669,10 +11654,10 @@
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
-        <v>888</v>
-      </c>
-      <c r="B19" s="141" t="s">
-        <v>889</v>
+        <v>882</v>
+      </c>
+      <c r="B19" s="142" t="s">
+        <v>883</v>
       </c>
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
@@ -11686,10 +11671,10 @@
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>890</v>
-      </c>
-      <c r="B20" s="141" t="s">
-        <v>891</v>
+        <v>884</v>
+      </c>
+      <c r="B20" s="142" t="s">
+        <v>885</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
@@ -11703,10 +11688,10 @@
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
-        <v>892</v>
+        <v>886</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>893</v>
+        <v>887</v>
       </c>
       <c r="C21" s="18"/>
       <c r="D21" s="18"/>
@@ -11720,10 +11705,10 @@
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>895</v>
+        <v>889</v>
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
@@ -11737,7 +11722,7 @@
     </row>
     <row r="23">
       <c r="A23" s="18"/>
-      <c r="B23" s="142"/>
+      <c r="B23" s="143"/>
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
@@ -11750,10 +11735,10 @@
     </row>
     <row r="24">
       <c r="A24" s="18" t="s">
-        <v>896</v>
-      </c>
-      <c r="B24" s="142" t="s">
-        <v>897</v>
+        <v>890</v>
+      </c>
+      <c r="B24" s="143" t="s">
+        <v>891</v>
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
@@ -11767,27 +11752,27 @@
     </row>
     <row r="25">
       <c r="A25" s="18" t="s">
-        <v>898</v>
+        <v>892</v>
       </c>
       <c r="B25" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="143"/>
-      <c r="D25" s="143"/>
-      <c r="E25" s="143"/>
-      <c r="F25" s="143"/>
-      <c r="G25" s="143"/>
-      <c r="H25" s="143"/>
-      <c r="I25" s="143"/>
-      <c r="J25" s="143"/>
-      <c r="K25" s="143"/>
+      <c r="C25" s="144"/>
+      <c r="D25" s="144"/>
+      <c r="E25" s="144"/>
+      <c r="F25" s="144"/>
+      <c r="G25" s="144"/>
+      <c r="H25" s="144"/>
+      <c r="I25" s="144"/>
+      <c r="J25" s="144"/>
+      <c r="K25" s="144"/>
     </row>
     <row r="26">
       <c r="A26" s="18" t="s">
-        <v>899</v>
+        <v>893</v>
       </c>
       <c r="B26" s="42" t="s">
-        <v>900</v>
+        <v>894</v>
       </c>
     </row>
     <row r="27">
@@ -11809,69 +11794,69 @@
       <c r="A32" s="18"/>
     </row>
     <row r="33">
-      <c r="A33" s="143" t="s">
-        <v>901</v>
-      </c>
-      <c r="B33" s="144" t="s">
-        <v>902</v>
+      <c r="A33" s="144" t="s">
+        <v>895</v>
+      </c>
+      <c r="B33" s="145" t="s">
+        <v>896</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="143" t="s">
-        <v>903</v>
-      </c>
-      <c r="B34" s="145" t="s">
-        <v>904</v>
-      </c>
-      <c r="C34" s="144"/>
-      <c r="D34" s="144"/>
-      <c r="E34" s="144"/>
-      <c r="F34" s="144"/>
-      <c r="G34" s="144"/>
-      <c r="H34" s="144"/>
-      <c r="I34" s="144"/>
-      <c r="J34" s="144"/>
-      <c r="K34" s="144"/>
+      <c r="A34" s="144" t="s">
+        <v>897</v>
+      </c>
+      <c r="B34" s="146" t="s">
+        <v>898</v>
+      </c>
+      <c r="C34" s="145"/>
+      <c r="D34" s="145"/>
+      <c r="E34" s="145"/>
+      <c r="F34" s="145"/>
+      <c r="G34" s="145"/>
+      <c r="H34" s="145"/>
+      <c r="I34" s="145"/>
+      <c r="J34" s="145"/>
+      <c r="K34" s="145"/>
     </row>
     <row r="35">
-      <c r="A35" s="143" t="s">
-        <v>905</v>
-      </c>
-      <c r="B35" s="145" t="s">
-        <v>906</v>
-      </c>
-      <c r="C35" s="146"/>
-      <c r="D35" s="146"/>
-      <c r="E35" s="146"/>
-      <c r="F35" s="146"/>
-      <c r="G35" s="146"/>
-      <c r="H35" s="146"/>
-      <c r="I35" s="146"/>
-      <c r="J35" s="146"/>
-      <c r="K35" s="146"/>
+      <c r="A35" s="144" t="s">
+        <v>899</v>
+      </c>
+      <c r="B35" s="146" t="s">
+        <v>900</v>
+      </c>
+      <c r="C35" s="147"/>
+      <c r="D35" s="147"/>
+      <c r="E35" s="147"/>
+      <c r="F35" s="147"/>
+      <c r="G35" s="147"/>
+      <c r="H35" s="147"/>
+      <c r="I35" s="147"/>
+      <c r="J35" s="147"/>
+      <c r="K35" s="147"/>
     </row>
     <row r="36">
       <c r="A36" s="18" t="s">
-        <v>907</v>
+        <v>901</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="18" t="s">
-        <v>908</v>
+        <v>902</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="18"/>
-      <c r="B38" s="143"/>
-      <c r="C38" s="143"/>
-      <c r="D38" s="143"/>
-      <c r="E38" s="143"/>
-      <c r="F38" s="143"/>
-      <c r="G38" s="143"/>
-      <c r="H38" s="143"/>
-      <c r="I38" s="143"/>
-      <c r="J38" s="143"/>
-      <c r="K38" s="143"/>
+      <c r="B38" s="144"/>
+      <c r="C38" s="144"/>
+      <c r="D38" s="144"/>
+      <c r="E38" s="144"/>
+      <c r="F38" s="144"/>
+      <c r="G38" s="144"/>
+      <c r="H38" s="144"/>
+      <c r="I38" s="144"/>
+      <c r="J38" s="144"/>
+      <c r="K38" s="144"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -11909,20 +11894,20 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="147" t="s">
+      <c r="A1" s="148" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="71" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="71" t="s">
-        <v>909</v>
+        <v>903</v>
       </c>
       <c r="D1" s="71" t="s">
-        <v>910</v>
+        <v>904</v>
       </c>
       <c r="E1" s="71" t="s">
-        <v>911</v>
+        <v>905</v>
       </c>
       <c r="F1" s="71" t="s">
         <v>10</v>
@@ -11933,10 +11918,10 @@
     </row>
     <row r="2">
       <c r="A2" s="15" t="s">
-        <v>912</v>
+        <v>906</v>
       </c>
       <c r="B2" s="40" t="s">
-        <v>913</v>
+        <v>907</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>361</v>
@@ -11952,10 +11937,10 @@
     </row>
     <row r="3">
       <c r="A3" s="15" t="s">
-        <v>914</v>
+        <v>908</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>915</v>
+        <v>909</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>375</v>
@@ -11971,10 +11956,10 @@
     </row>
     <row r="4">
       <c r="A4" s="15" t="s">
-        <v>916</v>
-      </c>
-      <c r="B4" s="148" t="s">
-        <v>917</v>
+        <v>910</v>
+      </c>
+      <c r="B4" s="149" t="s">
+        <v>911</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>391</v>
@@ -11986,14 +11971,14 @@
         <v>46</v>
       </c>
       <c r="F4" s="78"/>
-      <c r="G4" s="149"/>
+      <c r="G4" s="150"/>
     </row>
     <row r="5">
       <c r="A5" s="15" t="s">
-        <v>918</v>
-      </c>
-      <c r="B5" s="148" t="s">
-        <v>919</v>
+        <v>912</v>
+      </c>
+      <c r="B5" s="149" t="s">
+        <v>913</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>423</v>
@@ -12009,10 +11994,10 @@
     </row>
     <row r="6">
       <c r="A6" s="15" t="s">
-        <v>920</v>
-      </c>
-      <c r="B6" s="148" t="s">
-        <v>921</v>
+        <v>914</v>
+      </c>
+      <c r="B6" s="149" t="s">
+        <v>915</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>447</v>
@@ -12028,10 +12013,10 @@
     </row>
     <row r="7">
       <c r="A7" s="15" t="s">
-        <v>922</v>
-      </c>
-      <c r="B7" s="148" t="s">
-        <v>923</v>
+        <v>916</v>
+      </c>
+      <c r="B7" s="149" t="s">
+        <v>917</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>470</v>
@@ -12047,10 +12032,10 @@
     </row>
     <row r="8">
       <c r="A8" s="15" t="s">
-        <v>924</v>
-      </c>
-      <c r="B8" s="148" t="s">
-        <v>925</v>
+        <v>918</v>
+      </c>
+      <c r="B8" s="149" t="s">
+        <v>919</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>493</v>
@@ -12066,10 +12051,10 @@
     </row>
     <row r="9">
       <c r="A9" s="15" t="s">
-        <v>926</v>
-      </c>
-      <c r="B9" s="148" t="s">
-        <v>927</v>
+        <v>920</v>
+      </c>
+      <c r="B9" s="149" t="s">
+        <v>921</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>516</v>
@@ -12085,10 +12070,10 @@
     </row>
     <row r="10">
       <c r="A10" s="15" t="s">
-        <v>928</v>
-      </c>
-      <c r="B10" s="148" t="s">
-        <v>929</v>
+        <v>922</v>
+      </c>
+      <c r="B10" s="149" t="s">
+        <v>923</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>562</v>
@@ -12104,16 +12089,16 @@
     </row>
     <row r="11">
       <c r="A11" s="15" t="s">
-        <v>930</v>
-      </c>
-      <c r="B11" s="148" t="s">
-        <v>931</v>
+        <v>924</v>
+      </c>
+      <c r="B11" s="149" t="s">
+        <v>925</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="D11" s="109" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>270</v>
@@ -12123,16 +12108,16 @@
     </row>
     <row r="12">
       <c r="A12" s="15" t="s">
-        <v>932</v>
-      </c>
-      <c r="B12" s="148" t="s">
-        <v>933</v>
+        <v>926</v>
+      </c>
+      <c r="B12" s="149" t="s">
+        <v>927</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>273</v>
@@ -12142,16 +12127,16 @@
     </row>
     <row r="13">
       <c r="A13" s="15" t="s">
-        <v>934</v>
+        <v>928</v>
       </c>
       <c r="B13" s="40" t="s">
-        <v>935</v>
+        <v>929</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>276</v>
@@ -12161,16 +12146,16 @@
     </row>
     <row r="14">
       <c r="A14" s="15" t="s">
-        <v>936</v>
-      </c>
-      <c r="B14" s="148" t="s">
-        <v>937</v>
+        <v>930</v>
+      </c>
+      <c r="B14" s="149" t="s">
+        <v>931</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>279</v>
@@ -12180,16 +12165,16 @@
     </row>
     <row r="15">
       <c r="A15" s="15" t="s">
-        <v>938</v>
-      </c>
-      <c r="B15" s="148" t="s">
-        <v>939</v>
+        <v>932</v>
+      </c>
+      <c r="B15" s="149" t="s">
+        <v>933</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>282</v>
@@ -12199,16 +12184,16 @@
     </row>
     <row r="16">
       <c r="A16" s="15" t="s">
-        <v>940</v>
-      </c>
-      <c r="B16" s="148" t="s">
-        <v>941</v>
+        <v>934</v>
+      </c>
+      <c r="B16" s="149" t="s">
+        <v>935</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>647</v>
+        <v>641</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>285</v>
@@ -12218,16 +12203,16 @@
     </row>
     <row r="17">
       <c r="A17" s="15" t="s">
-        <v>942</v>
+        <v>936</v>
       </c>
       <c r="B17" s="40" t="s">
-        <v>943</v>
+        <v>937</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>655</v>
+        <v>649</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>288</v>
@@ -12237,16 +12222,16 @@
     </row>
     <row r="18">
       <c r="A18" s="15" t="s">
-        <v>944</v>
-      </c>
-      <c r="B18" s="148" t="s">
-        <v>945</v>
+        <v>938</v>
+      </c>
+      <c r="B18" s="149" t="s">
+        <v>939</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>662</v>
+        <v>656</v>
       </c>
       <c r="E18" s="15" t="s">
         <v>291</v>
@@ -12256,16 +12241,16 @@
     </row>
     <row r="19">
       <c r="A19" s="15" t="s">
-        <v>946</v>
-      </c>
-      <c r="B19" s="148" t="s">
-        <v>947</v>
+        <v>940</v>
+      </c>
+      <c r="B19" s="149" t="s">
+        <v>941</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>294</v>
@@ -12275,16 +12260,16 @@
     </row>
     <row r="20">
       <c r="A20" s="15" t="s">
-        <v>948</v>
-      </c>
-      <c r="B20" s="148" t="s">
-        <v>949</v>
+        <v>942</v>
+      </c>
+      <c r="B20" s="149" t="s">
+        <v>943</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>673</v>
+        <v>667</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>676</v>
+        <v>670</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>297</v>
@@ -12294,16 +12279,16 @@
     </row>
     <row r="21">
       <c r="A21" s="15" t="s">
-        <v>950</v>
-      </c>
-      <c r="B21" s="148" t="s">
-        <v>951</v>
+        <v>944</v>
+      </c>
+      <c r="B21" s="149" t="s">
+        <v>945</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>690</v>
+        <v>684</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>693</v>
+        <v>687</v>
       </c>
       <c r="E21" s="15" t="s">
         <v>300</v>
@@ -12313,16 +12298,16 @@
     </row>
     <row r="22">
       <c r="A22" s="15" t="s">
-        <v>952</v>
-      </c>
-      <c r="B22" s="148" t="s">
-        <v>953</v>
+        <v>946</v>
+      </c>
+      <c r="B22" s="149" t="s">
+        <v>947</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>705</v>
+        <v>699</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>708</v>
+        <v>702</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>303</v>
@@ -12332,16 +12317,16 @@
     </row>
     <row r="23">
       <c r="A23" s="15" t="s">
-        <v>954</v>
-      </c>
-      <c r="B23" s="148" t="s">
-        <v>955</v>
+        <v>948</v>
+      </c>
+      <c r="B23" s="149" t="s">
+        <v>949</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>714</v>
+        <v>708</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>717</v>
+        <v>711</v>
       </c>
       <c r="E23" s="15" t="s">
         <v>306</v>
@@ -12351,16 +12336,16 @@
     </row>
     <row r="24">
       <c r="A24" s="15" t="s">
-        <v>956</v>
-      </c>
-      <c r="B24" s="148" t="s">
-        <v>957</v>
+        <v>950</v>
+      </c>
+      <c r="B24" s="149" t="s">
+        <v>951</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>722</v>
+        <v>716</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>725</v>
+        <v>719</v>
       </c>
       <c r="E24" s="15" t="s">
         <v>309</v>
@@ -12370,16 +12355,16 @@
     </row>
     <row r="25">
       <c r="A25" s="15" t="s">
-        <v>958</v>
-      </c>
-      <c r="B25" s="148" t="s">
-        <v>959</v>
+        <v>952</v>
+      </c>
+      <c r="B25" s="149" t="s">
+        <v>953</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>731</v>
+        <v>725</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>734</v>
+        <v>728</v>
       </c>
       <c r="E25" s="15" t="s">
         <v>312</v>
@@ -12419,10 +12404,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="71" t="s">
-        <v>960</v>
+        <v>954</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>961</v>
+        <v>955</v>
       </c>
     </row>
     <row r="2">
@@ -12432,7 +12417,7 @@
       <c r="B2" s="73"/>
       <c r="C2" s="71"/>
       <c r="D2" s="4" t="s">
-        <v>962</v>
+        <v>956</v>
       </c>
       <c r="E2" s="22"/>
     </row>
@@ -12443,7 +12428,7 @@
       <c r="B3" s="71"/>
       <c r="C3" s="71"/>
       <c r="D3" s="4" t="s">
-        <v>963</v>
+        <v>957</v>
       </c>
       <c r="E3" s="22"/>
     </row>
@@ -12452,8 +12437,8 @@
         <v>343</v>
       </c>
       <c r="C4" s="71"/>
-      <c r="D4" s="141" t="s">
-        <v>964</v>
+      <c r="D4" s="142" t="s">
+        <v>958</v>
       </c>
       <c r="E4" s="22"/>
     </row>
@@ -12462,8 +12447,8 @@
         <v>344</v>
       </c>
       <c r="C5" s="71"/>
-      <c r="D5" s="141" t="s">
-        <v>965</v>
+      <c r="D5" s="142" t="s">
+        <v>959</v>
       </c>
       <c r="E5" s="22"/>
     </row>
@@ -12472,8 +12457,8 @@
         <v>349</v>
       </c>
       <c r="C6" s="71"/>
-      <c r="D6" s="141" t="s">
-        <v>966</v>
+      <c r="D6" s="142" t="s">
+        <v>960</v>
       </c>
       <c r="E6" s="22"/>
     </row>
@@ -12483,8 +12468,8 @@
       </c>
       <c r="B7" s="71"/>
       <c r="C7" s="71"/>
-      <c r="D7" s="141" t="s">
-        <v>967</v>
+      <c r="D7" s="142" t="s">
+        <v>961</v>
       </c>
       <c r="E7" s="22"/>
     </row>
@@ -12492,8 +12477,8 @@
       <c r="A8" s="16" t="s">
         <v>353</v>
       </c>
-      <c r="D8" s="141" t="s">
-        <v>968</v>
+      <c r="D8" s="142" t="s">
+        <v>962</v>
       </c>
     </row>
     <row r="9">
@@ -12502,8 +12487,8 @@
       </c>
       <c r="B9" s="71"/>
       <c r="C9" s="71"/>
-      <c r="D9" s="141" t="s">
-        <v>969</v>
+      <c r="D9" s="142" t="s">
+        <v>963</v>
       </c>
       <c r="E9" s="22"/>
     </row>
@@ -12539,416 +12524,416 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="150" t="s">
+      <c r="A1" s="151" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="150" t="s">
+      <c r="B1" s="151" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="151" t="s">
+      <c r="C1" s="152" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="150" t="s">
+      <c r="D1" s="151" t="s">
         <v>323</v>
       </c>
-      <c r="E1" s="150" t="s">
+      <c r="E1" s="151" t="s">
+        <v>964</v>
+      </c>
+      <c r="F1" s="151" t="s">
+        <v>965</v>
+      </c>
+      <c r="G1" s="152" t="s">
+        <v>966</v>
+      </c>
+      <c r="H1" s="153" t="s">
+        <v>967</v>
+      </c>
+      <c r="I1" s="154" t="s">
+        <v>332</v>
+      </c>
+      <c r="J1" s="155" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="154" t="s">
+        <v>258</v>
+      </c>
+      <c r="B2" s="154" t="s">
+        <v>969</v>
+      </c>
+      <c r="C2" s="154" t="s">
         <v>970</v>
       </c>
-      <c r="F1" s="150" t="s">
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="156"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="154"/>
+      <c r="J2" s="154" t="s">
         <v>971</v>
       </c>
-      <c r="G1" s="151" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="154" t="s">
+        <v>261</v>
+      </c>
+      <c r="B3" s="154" t="s">
         <v>972</v>
       </c>
-      <c r="H1" s="152" t="s">
+      <c r="C3" s="154" t="s">
         <v>973</v>
       </c>
-      <c r="I1" s="153" t="s">
-        <v>332</v>
-      </c>
-      <c r="J1" s="154" t="s">
+      <c r="D3" s="154"/>
+      <c r="E3" s="154"/>
+      <c r="F3" s="157"/>
+      <c r="G3" s="154"/>
+      <c r="H3" s="154"/>
+      <c r="I3" s="154"/>
+      <c r="J3" s="158" t="s">
         <v>974</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="153" t="s">
-        <v>258</v>
-      </c>
-      <c r="B2" s="153" t="s">
+    <row r="4">
+      <c r="A4" s="154" t="s">
+        <v>269</v>
+      </c>
+      <c r="B4" s="154" t="s">
         <v>975</v>
       </c>
-      <c r="C2" s="153" t="s">
+      <c r="C4" s="154" t="s">
         <v>976</v>
       </c>
-      <c r="D2" s="153"/>
-      <c r="E2" s="153"/>
-      <c r="F2" s="155"/>
-      <c r="G2" s="153"/>
-      <c r="H2" s="153"/>
-      <c r="I2" s="153"/>
-      <c r="J2" s="153" t="s">
+      <c r="D4" s="154"/>
+      <c r="E4" s="159"/>
+      <c r="F4" s="157"/>
+      <c r="G4" s="154"/>
+      <c r="H4" s="154"/>
+      <c r="I4" s="154"/>
+      <c r="J4" s="154" t="s">
         <v>977</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="153" t="s">
-        <v>261</v>
-      </c>
-      <c r="B3" s="153" t="s">
+    <row r="5">
+      <c r="A5" s="154" t="s">
+        <v>272</v>
+      </c>
+      <c r="B5" s="154" t="s">
         <v>978</v>
       </c>
-      <c r="C3" s="153" t="s">
+      <c r="C5" s="154" t="s">
         <v>979</v>
       </c>
-      <c r="D3" s="153"/>
-      <c r="E3" s="153"/>
-      <c r="F3" s="156"/>
-      <c r="G3" s="153"/>
-      <c r="H3" s="153"/>
-      <c r="I3" s="153"/>
-      <c r="J3" s="157" t="s">
+      <c r="D5" s="160"/>
+      <c r="E5" s="159"/>
+      <c r="F5" s="156"/>
+      <c r="G5" s="154"/>
+      <c r="H5" s="154"/>
+      <c r="I5" s="154"/>
+      <c r="J5" s="154" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="154" t="s">
+        <v>275</v>
+      </c>
+      <c r="B6" s="154" t="s">
         <v>980</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="153" t="s">
-        <v>269</v>
-      </c>
-      <c r="B4" s="153" t="s">
+      <c r="C6" s="154" t="s">
         <v>981</v>
       </c>
-      <c r="C4" s="153" t="s">
+      <c r="D6" s="154"/>
+      <c r="E6" s="159"/>
+      <c r="F6" s="156"/>
+      <c r="G6" s="154"/>
+      <c r="H6" s="154"/>
+      <c r="I6" s="154"/>
+      <c r="J6" s="154" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="154" t="s">
+        <v>278</v>
+      </c>
+      <c r="B7" s="154" t="s">
         <v>982</v>
       </c>
-      <c r="D4" s="153"/>
-      <c r="E4" s="158"/>
-      <c r="F4" s="156"/>
-      <c r="G4" s="153"/>
-      <c r="H4" s="153"/>
-      <c r="I4" s="153"/>
-      <c r="J4" s="153" t="s">
+      <c r="C7" s="154" t="s">
         <v>983</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="153" t="s">
-        <v>272</v>
-      </c>
-      <c r="B5" s="153" t="s">
+      <c r="D7" s="154"/>
+      <c r="E7" s="159"/>
+      <c r="F7" s="156"/>
+      <c r="G7" s="154"/>
+      <c r="H7" s="154"/>
+      <c r="I7" s="154"/>
+      <c r="J7" s="154" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="154" t="s">
+        <v>281</v>
+      </c>
+      <c r="B8" s="154" t="s">
         <v>984</v>
       </c>
-      <c r="C5" s="153" t="s">
+      <c r="C8" s="154" t="s">
         <v>985</v>
       </c>
-      <c r="D5" s="159"/>
-      <c r="E5" s="158"/>
-      <c r="F5" s="155"/>
-      <c r="G5" s="153"/>
-      <c r="H5" s="153"/>
-      <c r="I5" s="153"/>
-      <c r="J5" s="153" t="s">
-        <v>983</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="153" t="s">
-        <v>275</v>
-      </c>
-      <c r="B6" s="153" t="s">
+      <c r="D8" s="160"/>
+      <c r="E8" s="159"/>
+      <c r="F8" s="156"/>
+      <c r="G8" s="154"/>
+      <c r="H8" s="154"/>
+      <c r="I8" s="153"/>
+      <c r="J8" s="161" t="s">
         <v>986</v>
       </c>
-      <c r="C6" s="153" t="s">
+    </row>
+    <row r="9">
+      <c r="A9" s="154" t="s">
+        <v>284</v>
+      </c>
+      <c r="B9" s="154" t="s">
         <v>987</v>
       </c>
-      <c r="D6" s="153"/>
-      <c r="E6" s="158"/>
-      <c r="F6" s="155"/>
-      <c r="G6" s="153"/>
-      <c r="H6" s="153"/>
-      <c r="I6" s="153"/>
-      <c r="J6" s="153" t="s">
-        <v>983</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="153" t="s">
-        <v>278</v>
-      </c>
-      <c r="B7" s="153" t="s">
+      <c r="C9" s="154" t="s">
         <v>988</v>
       </c>
-      <c r="C7" s="153" t="s">
+      <c r="D9" s="154"/>
+      <c r="E9" s="159"/>
+      <c r="F9" s="156"/>
+      <c r="G9" s="154"/>
+      <c r="H9" s="154"/>
+      <c r="I9" s="154"/>
+      <c r="J9" s="162" t="s">
         <v>989</v>
       </c>
-      <c r="D7" s="153"/>
-      <c r="E7" s="158"/>
-      <c r="F7" s="155"/>
-      <c r="G7" s="153"/>
-      <c r="H7" s="153"/>
-      <c r="I7" s="153"/>
-      <c r="J7" s="153" t="s">
-        <v>983</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="153" t="s">
-        <v>281</v>
-      </c>
-      <c r="B8" s="153" t="s">
+    </row>
+    <row r="10">
+      <c r="A10" s="154" t="s">
+        <v>287</v>
+      </c>
+      <c r="B10" s="154" t="s">
         <v>990</v>
       </c>
-      <c r="C8" s="153" t="s">
+      <c r="C10" s="154" t="s">
         <v>991</v>
       </c>
-      <c r="D8" s="159"/>
-      <c r="E8" s="158"/>
-      <c r="F8" s="155"/>
-      <c r="G8" s="153"/>
-      <c r="H8" s="153"/>
-      <c r="I8" s="152"/>
-      <c r="J8" s="160" t="s">
+      <c r="D10" s="154"/>
+      <c r="E10" s="159"/>
+      <c r="F10" s="156"/>
+      <c r="G10" s="154"/>
+      <c r="H10" s="154"/>
+      <c r="I10" s="154"/>
+      <c r="J10" s="162" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="154" t="s">
+        <v>290</v>
+      </c>
+      <c r="B11" s="154" t="s">
         <v>992</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="153" t="s">
-        <v>284</v>
-      </c>
-      <c r="B9" s="153" t="s">
+      <c r="C11" s="154" t="s">
         <v>993</v>
       </c>
-      <c r="C9" s="153" t="s">
+      <c r="D11" s="154"/>
+      <c r="E11" s="159"/>
+      <c r="F11" s="157"/>
+      <c r="G11" s="154"/>
+      <c r="H11" s="154"/>
+      <c r="I11" s="154"/>
+      <c r="J11" s="161" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="154" t="s">
+        <v>293</v>
+      </c>
+      <c r="B12" s="154" t="s">
         <v>994</v>
       </c>
-      <c r="D9" s="153"/>
-      <c r="E9" s="158"/>
-      <c r="F9" s="155"/>
-      <c r="G9" s="153"/>
-      <c r="H9" s="153"/>
-      <c r="I9" s="153"/>
-      <c r="J9" s="161" t="s">
+      <c r="C12" s="154" t="s">
         <v>995</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="153" t="s">
-        <v>287</v>
-      </c>
-      <c r="B10" s="153" t="s">
+      <c r="D12" s="154"/>
+      <c r="E12" s="159"/>
+      <c r="F12" s="156"/>
+      <c r="G12" s="154"/>
+      <c r="H12" s="154"/>
+      <c r="I12" s="16" t="s">
         <v>996</v>
       </c>
-      <c r="C10" s="153" t="s">
+      <c r="J12" s="158" t="s">
         <v>997</v>
       </c>
-      <c r="D10" s="153"/>
-      <c r="E10" s="158"/>
-      <c r="F10" s="155"/>
-      <c r="G10" s="153"/>
-      <c r="H10" s="153"/>
-      <c r="I10" s="153"/>
-      <c r="J10" s="161" t="s">
-        <v>995</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="153" t="s">
-        <v>290</v>
-      </c>
-      <c r="B11" s="153" t="s">
+    </row>
+    <row r="13">
+      <c r="A13" s="154" t="s">
+        <v>296</v>
+      </c>
+      <c r="B13" s="154" t="s">
         <v>998</v>
       </c>
-      <c r="C11" s="153" t="s">
+      <c r="C13" s="154" t="s">
         <v>999</v>
       </c>
-      <c r="D11" s="153"/>
-      <c r="E11" s="158"/>
-      <c r="F11" s="156"/>
-      <c r="G11" s="153"/>
-      <c r="H11" s="153"/>
-      <c r="I11" s="153"/>
-      <c r="J11" s="160" t="s">
-        <v>992</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="153" t="s">
-        <v>293</v>
-      </c>
-      <c r="B12" s="153" t="s">
+      <c r="D13" s="154"/>
+      <c r="E13" s="159"/>
+      <c r="F13" s="157"/>
+      <c r="G13" s="154"/>
+      <c r="H13" s="154"/>
+      <c r="I13" s="16" t="s">
+        <v>996</v>
+      </c>
+      <c r="J13" s="158" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="154" t="s">
+        <v>299</v>
+      </c>
+      <c r="B14" s="154" t="s">
         <v>1000</v>
       </c>
-      <c r="C12" s="153" t="s">
+      <c r="C14" s="154" t="s">
         <v>1001</v>
       </c>
-      <c r="D12" s="153"/>
-      <c r="E12" s="158"/>
-      <c r="F12" s="155"/>
-      <c r="G12" s="153"/>
-      <c r="H12" s="153"/>
-      <c r="I12" s="16" t="s">
+      <c r="D14" s="154"/>
+      <c r="E14" s="159"/>
+      <c r="F14" s="157"/>
+      <c r="G14" s="154"/>
+      <c r="H14" s="154"/>
+      <c r="J14" s="161" t="s">
         <v>1002</v>
       </c>
-      <c r="J12" s="157" t="s">
+    </row>
+    <row r="15">
+      <c r="A15" s="154" t="s">
+        <v>302</v>
+      </c>
+      <c r="B15" s="154" t="s">
         <v>1003</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="153" t="s">
-        <v>296</v>
-      </c>
-      <c r="B13" s="153" t="s">
+      <c r="C15" s="154" t="s">
         <v>1004</v>
       </c>
-      <c r="C13" s="153" t="s">
+      <c r="D15" s="154"/>
+      <c r="E15" s="159"/>
+      <c r="F15" s="157"/>
+      <c r="G15" s="154"/>
+      <c r="H15" s="154"/>
+      <c r="J15" s="161" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="154" t="s">
+        <v>305</v>
+      </c>
+      <c r="B16" s="154" t="s">
         <v>1005</v>
       </c>
-      <c r="D13" s="153"/>
-      <c r="E13" s="158"/>
-      <c r="F13" s="156"/>
-      <c r="G13" s="153"/>
-      <c r="H13" s="153"/>
-      <c r="I13" s="16" t="s">
-        <v>1002</v>
-      </c>
-      <c r="J13" s="157" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="153" t="s">
-        <v>299</v>
-      </c>
-      <c r="B14" s="153" t="s">
+      <c r="C16" s="154" t="s">
         <v>1006</v>
       </c>
-      <c r="C14" s="153" t="s">
+      <c r="D16" s="154"/>
+      <c r="E16" s="159"/>
+      <c r="F16" s="157"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154" t="s">
         <v>1007</v>
       </c>
-      <c r="D14" s="153"/>
-      <c r="E14" s="158"/>
-      <c r="F14" s="156"/>
-      <c r="G14" s="153"/>
-      <c r="H14" s="153"/>
-      <c r="J14" s="160" t="s">
+    </row>
+    <row r="17">
+      <c r="A17" s="154" t="s">
+        <v>308</v>
+      </c>
+      <c r="B17" s="154" t="s">
         <v>1008</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="153" t="s">
-        <v>302</v>
-      </c>
-      <c r="B15" s="153" t="s">
+      <c r="C17" s="154" t="s">
         <v>1009</v>
       </c>
-      <c r="C15" s="153" t="s">
+      <c r="D17" s="154"/>
+      <c r="E17" s="159"/>
+      <c r="F17" s="156"/>
+      <c r="G17" s="154"/>
+      <c r="H17" s="154"/>
+      <c r="I17" s="153"/>
+      <c r="J17" s="163" t="s">
         <v>1010</v>
       </c>
-      <c r="D15" s="153"/>
-      <c r="E15" s="158"/>
-      <c r="F15" s="156"/>
-      <c r="G15" s="153"/>
-      <c r="H15" s="153"/>
-      <c r="J15" s="160" t="s">
-        <v>1008</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="153" t="s">
-        <v>305</v>
-      </c>
-      <c r="B16" s="153" t="s">
+    </row>
+    <row r="18">
+      <c r="A18" s="154" t="s">
+        <v>311</v>
+      </c>
+      <c r="B18" s="154" t="s">
         <v>1011</v>
       </c>
-      <c r="C16" s="153" t="s">
+      <c r="C18" s="154" t="s">
         <v>1012</v>
       </c>
-      <c r="D16" s="153"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="156"/>
-      <c r="G16" s="153"/>
-      <c r="H16" s="153"/>
-      <c r="I16" s="153"/>
-      <c r="J16" s="153" t="s">
+      <c r="D18" s="154"/>
+      <c r="E18" s="159"/>
+      <c r="F18" s="156"/>
+      <c r="G18" s="154"/>
+      <c r="H18" s="154"/>
+      <c r="I18" s="153"/>
+      <c r="J18" s="163" t="s">
         <v>1013</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="153" t="s">
-        <v>308</v>
-      </c>
-      <c r="B17" s="153" t="s">
+    <row r="19">
+      <c r="A19" s="154" t="s">
+        <v>314</v>
+      </c>
+      <c r="B19" s="154" t="s">
         <v>1014</v>
       </c>
-      <c r="C17" s="153" t="s">
+      <c r="C19" s="154" t="s">
         <v>1015</v>
       </c>
-      <c r="D17" s="153"/>
-      <c r="E17" s="158"/>
-      <c r="F17" s="155"/>
-      <c r="G17" s="153"/>
-      <c r="H17" s="153"/>
-      <c r="I17" s="152"/>
-      <c r="J17" s="162" t="s">
+      <c r="D19" s="154"/>
+      <c r="E19" s="159"/>
+      <c r="F19" s="156"/>
+      <c r="G19" s="154"/>
+      <c r="H19" s="154"/>
+      <c r="I19" s="153"/>
+      <c r="J19" s="163" t="s">
         <v>1016</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="153" t="s">
-        <v>311</v>
-      </c>
-      <c r="B18" s="153" t="s">
+    <row r="20">
+      <c r="A20" s="159" t="s">
         <v>1017</v>
       </c>
-      <c r="C18" s="153" t="s">
+      <c r="B20" s="154" t="s">
         <v>1018</v>
       </c>
-      <c r="D18" s="153"/>
-      <c r="E18" s="158"/>
-      <c r="F18" s="155"/>
-      <c r="G18" s="153"/>
-      <c r="H18" s="153"/>
-      <c r="I18" s="152"/>
-      <c r="J18" s="162" t="s">
-        <v>1019</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="153" t="s">
-        <v>314</v>
-      </c>
-      <c r="B19" s="153" t="s">
-        <v>1020</v>
-      </c>
-      <c r="C19" s="153" t="s">
-        <v>1021</v>
-      </c>
-      <c r="D19" s="153"/>
-      <c r="E19" s="158"/>
-      <c r="F19" s="155"/>
-      <c r="G19" s="153"/>
-      <c r="H19" s="153"/>
-      <c r="I19" s="152"/>
-      <c r="J19" s="162" t="s">
-        <v>1022</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="158" t="s">
-        <v>1023</v>
-      </c>
-      <c r="B20" s="153" t="s">
-        <v>1024</v>
-      </c>
-      <c r="C20" s="158"/>
-      <c r="D20" s="158" t="s">
+      <c r="C20" s="159"/>
+      <c r="D20" s="159" t="s">
         <v>151</v>
       </c>
-      <c r="E20" s="158"/>
-      <c r="F20" s="155"/>
-      <c r="G20" s="153"/>
-      <c r="H20" s="153"/>
-      <c r="I20" s="152"/>
-      <c r="J20" s="152"/>
+      <c r="E20" s="159"/>
+      <c r="F20" s="156"/>
+      <c r="G20" s="154"/>
+      <c r="H20" s="154"/>
+      <c r="I20" s="153"/>
+      <c r="J20" s="153"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -12976,53 +12961,53 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1025</v>
+        <v>1019</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1026</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="16" t="s">
-        <v>1027</v>
-      </c>
-      <c r="C2" s="163" t="s">
-        <v>1028</v>
+        <v>1021</v>
+      </c>
+      <c r="C2" s="164" t="s">
+        <v>1022</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="16" t="s">
-        <v>1029</v>
-      </c>
-      <c r="C3" s="163" t="s">
-        <v>1030</v>
+        <v>1023</v>
+      </c>
+      <c r="C3" s="164" t="s">
+        <v>1024</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="16" t="s">
-        <v>1031</v>
-      </c>
-      <c r="C4" s="163" t="s">
-        <v>1032</v>
+        <v>1025</v>
+      </c>
+      <c r="C4" s="164" t="s">
+        <v>1026</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="16" t="s">
-        <v>1033</v>
-      </c>
-      <c r="C5" s="163" t="s">
-        <v>1034</v>
+        <v>1027</v>
+      </c>
+      <c r="C5" s="164" t="s">
+        <v>1028</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="16" t="s">
-        <v>1002</v>
+        <v>996</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>1035</v>
-      </c>
-      <c r="C6" s="163" t="s">
-        <v>1036</v>
+        <v>1029</v>
+      </c>
+      <c r="C6" s="164" t="s">
+        <v>1030</v>
       </c>
     </row>
   </sheetData>

</xml_diff>